<commit_message>
Updated the VV PIIDs
</commit_message>
<xml_diff>
--- a/PIID/VV.xlsx
+++ b/PIID/VV.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="52">
   <si>
     <t>V&amp;V</t>
   </si>
@@ -188,7 +188,10 @@
     <t>OBH012 Detailed Validation Report</t>
   </si>
   <si>
-    <t>Defect analysis in Metrics Report</t>
+    <t>8D CAPA used to analyzed the one critical validation defect.</t>
+  </si>
+  <si>
+    <t>OBH012_ROCSAN</t>
   </si>
 </sst>
 </file>
@@ -307,18 +310,12 @@
       <charset val="134"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
   </fills>
   <borders count="10">
@@ -446,7 +443,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -622,6 +619,30 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -634,33 +655,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -668,63 +662,7 @@
     <cellStyle name="Normal 2" xfId="2"/>
     <cellStyle name="Normal 2 2" xfId="3"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="25">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1173,10 +1111,10 @@
   <dimension ref="A1:R276"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D91" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" sqref="A1:F2"/>
+      <selection pane="bottomRight" activeCell="E95" sqref="E95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75"/>
@@ -1193,25 +1131,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18">
-      <c r="A1" s="61" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
+      <c r="E1" s="70"/>
+      <c r="F1" s="70"/>
       <c r="L1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:18">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="64"/>
+      <c r="A2" s="71"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="72"/>
     </row>
     <row r="3" spans="1:18" s="1" customFormat="1" ht="71.25">
       <c r="A3" s="3" t="s">
@@ -1264,7 +1202,7 @@
       <c r="B4" s="59">
         <v>1.1000000000000001</v>
       </c>
-      <c r="C4" s="72" t="s">
+      <c r="C4" s="65" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="5" t="str">
@@ -1301,13 +1239,13 @@
       <c r="N4" s="7"/>
       <c r="O4" s="7"/>
       <c r="P4" s="7"/>
-      <c r="Q4" s="69"/>
+      <c r="Q4" s="66"/>
       <c r="R4" s="59"/>
     </row>
     <row r="5" spans="1:18" ht="51">
       <c r="A5" s="59"/>
       <c r="B5" s="59"/>
-      <c r="C5" s="72"/>
+      <c r="C5" s="65"/>
       <c r="D5" s="5" t="str">
         <f t="shared" ref="D5:D68" si="2">IF(LEN(E5)&gt;5,IF(LEN(K5&amp;L5&amp;M5)&gt;=1,"OK","Check"),"-")</f>
         <v>OK</v>
@@ -1342,13 +1280,13 @@
       <c r="N5" s="7"/>
       <c r="O5" s="7"/>
       <c r="P5" s="7"/>
-      <c r="Q5" s="70"/>
+      <c r="Q5" s="67"/>
       <c r="R5" s="59"/>
     </row>
     <row r="6" spans="1:18" ht="15.75">
       <c r="A6" s="59"/>
       <c r="B6" s="59"/>
-      <c r="C6" s="72"/>
+      <c r="C6" s="65"/>
       <c r="D6" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1377,13 +1315,13 @@
       <c r="N6" s="7"/>
       <c r="O6" s="7"/>
       <c r="P6" s="7"/>
-      <c r="Q6" s="70"/>
+      <c r="Q6" s="67"/>
       <c r="R6" s="59"/>
     </row>
     <row r="7" spans="1:18" ht="15.75">
       <c r="A7" s="59"/>
       <c r="B7" s="59"/>
-      <c r="C7" s="72"/>
+      <c r="C7" s="65"/>
       <c r="D7" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1412,13 +1350,13 @@
       <c r="N7" s="7"/>
       <c r="O7" s="7"/>
       <c r="P7" s="7"/>
-      <c r="Q7" s="70"/>
+      <c r="Q7" s="67"/>
       <c r="R7" s="59"/>
     </row>
     <row r="8" spans="1:18" ht="15.75">
       <c r="A8" s="59"/>
       <c r="B8" s="59"/>
-      <c r="C8" s="72"/>
+      <c r="C8" s="65"/>
       <c r="D8" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1447,13 +1385,13 @@
       <c r="N8" s="7"/>
       <c r="O8" s="7"/>
       <c r="P8" s="7"/>
-      <c r="Q8" s="70"/>
+      <c r="Q8" s="67"/>
       <c r="R8" s="59"/>
     </row>
     <row r="9" spans="1:18" ht="15.75">
       <c r="A9" s="59"/>
       <c r="B9" s="59"/>
-      <c r="C9" s="72"/>
+      <c r="C9" s="65"/>
       <c r="D9" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1482,13 +1420,13 @@
       <c r="N9" s="7"/>
       <c r="O9" s="7"/>
       <c r="P9" s="7"/>
-      <c r="Q9" s="70"/>
+      <c r="Q9" s="67"/>
       <c r="R9" s="59"/>
     </row>
     <row r="10" spans="1:18" ht="15.75">
       <c r="A10" s="59"/>
       <c r="B10" s="59"/>
-      <c r="C10" s="72"/>
+      <c r="C10" s="65"/>
       <c r="D10" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1517,13 +1455,13 @@
       <c r="N10" s="7"/>
       <c r="O10" s="7"/>
       <c r="P10" s="7"/>
-      <c r="Q10" s="70"/>
+      <c r="Q10" s="67"/>
       <c r="R10" s="59"/>
     </row>
     <row r="11" spans="1:18" ht="30" customHeight="1">
       <c r="A11" s="59"/>
       <c r="B11" s="59"/>
-      <c r="C11" s="72"/>
+      <c r="C11" s="65"/>
       <c r="D11" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1552,13 +1490,13 @@
       <c r="N11" s="7"/>
       <c r="O11" s="7"/>
       <c r="P11" s="7"/>
-      <c r="Q11" s="70"/>
+      <c r="Q11" s="67"/>
       <c r="R11" s="59"/>
     </row>
     <row r="12" spans="1:18" ht="15.75">
       <c r="A12" s="59"/>
       <c r="B12" s="59"/>
-      <c r="C12" s="72"/>
+      <c r="C12" s="65"/>
       <c r="D12" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1587,13 +1525,13 @@
       <c r="N12" s="7"/>
       <c r="O12" s="7"/>
       <c r="P12" s="7"/>
-      <c r="Q12" s="70"/>
+      <c r="Q12" s="67"/>
       <c r="R12" s="59"/>
     </row>
     <row r="13" spans="1:18" ht="15.75">
       <c r="A13" s="59"/>
       <c r="B13" s="59"/>
-      <c r="C13" s="72"/>
+      <c r="C13" s="65"/>
       <c r="D13" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1622,13 +1560,13 @@
       <c r="N13" s="7"/>
       <c r="O13" s="7"/>
       <c r="P13" s="7"/>
-      <c r="Q13" s="70"/>
+      <c r="Q13" s="67"/>
       <c r="R13" s="59"/>
     </row>
     <row r="14" spans="1:18" ht="15.75">
       <c r="A14" s="59"/>
       <c r="B14" s="59"/>
-      <c r="C14" s="72"/>
+      <c r="C14" s="65"/>
       <c r="D14" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1657,13 +1595,13 @@
       <c r="N14" s="7"/>
       <c r="O14" s="7"/>
       <c r="P14" s="7"/>
-      <c r="Q14" s="70"/>
+      <c r="Q14" s="67"/>
       <c r="R14" s="59"/>
     </row>
     <row r="15" spans="1:18" ht="15.75">
       <c r="A15" s="59"/>
       <c r="B15" s="59"/>
-      <c r="C15" s="72"/>
+      <c r="C15" s="65"/>
       <c r="D15" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1692,13 +1630,13 @@
       <c r="N15" s="7"/>
       <c r="O15" s="7"/>
       <c r="P15" s="7"/>
-      <c r="Q15" s="70"/>
+      <c r="Q15" s="67"/>
       <c r="R15" s="59"/>
     </row>
     <row r="16" spans="1:18" ht="15.75">
       <c r="A16" s="59"/>
       <c r="B16" s="59"/>
-      <c r="C16" s="72"/>
+      <c r="C16" s="65"/>
       <c r="D16" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1727,13 +1665,13 @@
       <c r="N16" s="7"/>
       <c r="O16" s="7"/>
       <c r="P16" s="7"/>
-      <c r="Q16" s="70"/>
+      <c r="Q16" s="67"/>
       <c r="R16" s="59"/>
     </row>
     <row r="17" spans="1:18" ht="15.75">
       <c r="A17" s="59"/>
       <c r="B17" s="59"/>
-      <c r="C17" s="72"/>
+      <c r="C17" s="65"/>
       <c r="D17" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1762,13 +1700,13 @@
       <c r="N17" s="7"/>
       <c r="O17" s="7"/>
       <c r="P17" s="7"/>
-      <c r="Q17" s="70"/>
+      <c r="Q17" s="67"/>
       <c r="R17" s="59"/>
     </row>
     <row r="18" spans="1:18" ht="15.75">
       <c r="A18" s="59"/>
       <c r="B18" s="59"/>
-      <c r="C18" s="72"/>
+      <c r="C18" s="65"/>
       <c r="D18" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1797,7 +1735,7 @@
       <c r="N18" s="7"/>
       <c r="O18" s="7"/>
       <c r="P18" s="7"/>
-      <c r="Q18" s="71"/>
+      <c r="Q18" s="68"/>
       <c r="R18" s="59"/>
     </row>
     <row r="19" spans="1:18" ht="51">
@@ -1805,7 +1743,7 @@
       <c r="B19" s="59">
         <v>1.2</v>
       </c>
-      <c r="C19" s="72" t="s">
+      <c r="C19" s="65" t="s">
         <v>15</v>
       </c>
       <c r="D19" s="5" t="str">
@@ -1842,13 +1780,13 @@
       <c r="N19" s="7"/>
       <c r="O19" s="7"/>
       <c r="P19" s="7"/>
-      <c r="Q19" s="69"/>
+      <c r="Q19" s="66"/>
       <c r="R19" s="59"/>
     </row>
     <row r="20" spans="1:18" ht="38.25">
       <c r="A20" s="59"/>
       <c r="B20" s="59"/>
-      <c r="C20" s="72"/>
+      <c r="C20" s="65"/>
       <c r="D20" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -1883,13 +1821,13 @@
       <c r="N20" s="7"/>
       <c r="O20" s="7"/>
       <c r="P20" s="7"/>
-      <c r="Q20" s="70"/>
+      <c r="Q20" s="67"/>
       <c r="R20" s="59"/>
     </row>
     <row r="21" spans="1:18" ht="15.75">
       <c r="A21" s="59"/>
       <c r="B21" s="59"/>
-      <c r="C21" s="72"/>
+      <c r="C21" s="65"/>
       <c r="D21" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1918,13 +1856,13 @@
       <c r="N21" s="7"/>
       <c r="O21" s="7"/>
       <c r="P21" s="7"/>
-      <c r="Q21" s="70"/>
+      <c r="Q21" s="67"/>
       <c r="R21" s="59"/>
     </row>
     <row r="22" spans="1:18" ht="15.75">
       <c r="A22" s="59"/>
       <c r="B22" s="59"/>
-      <c r="C22" s="72"/>
+      <c r="C22" s="65"/>
       <c r="D22" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1953,13 +1891,13 @@
       <c r="N22" s="7"/>
       <c r="O22" s="7"/>
       <c r="P22" s="7"/>
-      <c r="Q22" s="70"/>
+      <c r="Q22" s="67"/>
       <c r="R22" s="59"/>
     </row>
     <row r="23" spans="1:18" ht="15.75">
       <c r="A23" s="59"/>
       <c r="B23" s="59"/>
-      <c r="C23" s="72"/>
+      <c r="C23" s="65"/>
       <c r="D23" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -1988,13 +1926,13 @@
       <c r="N23" s="7"/>
       <c r="O23" s="7"/>
       <c r="P23" s="7"/>
-      <c r="Q23" s="70"/>
+      <c r="Q23" s="67"/>
       <c r="R23" s="59"/>
     </row>
     <row r="24" spans="1:18" ht="15.75">
       <c r="A24" s="59"/>
       <c r="B24" s="59"/>
-      <c r="C24" s="72"/>
+      <c r="C24" s="65"/>
       <c r="D24" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2023,13 +1961,13 @@
       <c r="N24" s="7"/>
       <c r="O24" s="7"/>
       <c r="P24" s="7"/>
-      <c r="Q24" s="70"/>
+      <c r="Q24" s="67"/>
       <c r="R24" s="59"/>
     </row>
     <row r="25" spans="1:18" ht="15.75">
       <c r="A25" s="59"/>
       <c r="B25" s="59"/>
-      <c r="C25" s="72"/>
+      <c r="C25" s="65"/>
       <c r="D25" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2058,13 +1996,13 @@
       <c r="N25" s="7"/>
       <c r="O25" s="7"/>
       <c r="P25" s="7"/>
-      <c r="Q25" s="70"/>
+      <c r="Q25" s="67"/>
       <c r="R25" s="59"/>
     </row>
     <row r="26" spans="1:18" ht="26.25" customHeight="1">
       <c r="A26" s="59"/>
       <c r="B26" s="59"/>
-      <c r="C26" s="72"/>
+      <c r="C26" s="65"/>
       <c r="D26" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2093,13 +2031,13 @@
       <c r="N26" s="7"/>
       <c r="O26" s="7"/>
       <c r="P26" s="7"/>
-      <c r="Q26" s="70"/>
+      <c r="Q26" s="67"/>
       <c r="R26" s="59"/>
     </row>
     <row r="27" spans="1:18" ht="15.75">
       <c r="A27" s="59"/>
       <c r="B27" s="59"/>
-      <c r="C27" s="72"/>
+      <c r="C27" s="65"/>
       <c r="D27" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2128,13 +2066,13 @@
       <c r="N27" s="10"/>
       <c r="O27" s="10"/>
       <c r="P27" s="10"/>
-      <c r="Q27" s="70"/>
+      <c r="Q27" s="67"/>
       <c r="R27" s="59"/>
     </row>
     <row r="28" spans="1:18" ht="15.75">
       <c r="A28" s="59"/>
       <c r="B28" s="59"/>
-      <c r="C28" s="72"/>
+      <c r="C28" s="65"/>
       <c r="D28" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2163,13 +2101,13 @@
       <c r="N28" s="10"/>
       <c r="O28" s="10"/>
       <c r="P28" s="10"/>
-      <c r="Q28" s="70"/>
+      <c r="Q28" s="67"/>
       <c r="R28" s="59"/>
     </row>
     <row r="29" spans="1:18" ht="15.75">
       <c r="A29" s="59"/>
       <c r="B29" s="59"/>
-      <c r="C29" s="72"/>
+      <c r="C29" s="65"/>
       <c r="D29" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2198,13 +2136,13 @@
       <c r="N29" s="10"/>
       <c r="O29" s="10"/>
       <c r="P29" s="10"/>
-      <c r="Q29" s="70"/>
+      <c r="Q29" s="67"/>
       <c r="R29" s="59"/>
     </row>
     <row r="30" spans="1:18" ht="15.75">
       <c r="A30" s="59"/>
       <c r="B30" s="59"/>
-      <c r="C30" s="72"/>
+      <c r="C30" s="65"/>
       <c r="D30" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2233,13 +2171,13 @@
       <c r="N30" s="10"/>
       <c r="O30" s="10"/>
       <c r="P30" s="10"/>
-      <c r="Q30" s="70"/>
+      <c r="Q30" s="67"/>
       <c r="R30" s="59"/>
     </row>
     <row r="31" spans="1:18" ht="15.75">
       <c r="A31" s="59"/>
       <c r="B31" s="59"/>
-      <c r="C31" s="72"/>
+      <c r="C31" s="65"/>
       <c r="D31" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2268,13 +2206,13 @@
       <c r="N31" s="10"/>
       <c r="O31" s="10"/>
       <c r="P31" s="10"/>
-      <c r="Q31" s="70"/>
+      <c r="Q31" s="67"/>
       <c r="R31" s="59"/>
     </row>
     <row r="32" spans="1:18" ht="15.75">
       <c r="A32" s="59"/>
       <c r="B32" s="59"/>
-      <c r="C32" s="72"/>
+      <c r="C32" s="65"/>
       <c r="D32" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2303,13 +2241,13 @@
       <c r="N32" s="10"/>
       <c r="O32" s="10"/>
       <c r="P32" s="10"/>
-      <c r="Q32" s="70"/>
+      <c r="Q32" s="67"/>
       <c r="R32" s="59"/>
     </row>
     <row r="33" spans="1:18" ht="15.75">
       <c r="A33" s="59"/>
       <c r="B33" s="59"/>
-      <c r="C33" s="72"/>
+      <c r="C33" s="65"/>
       <c r="D33" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2338,7 +2276,7 @@
       <c r="N33" s="10"/>
       <c r="O33" s="10"/>
       <c r="P33" s="10"/>
-      <c r="Q33" s="71"/>
+      <c r="Q33" s="68"/>
       <c r="R33" s="59"/>
     </row>
     <row r="34" spans="1:18" ht="38.25" customHeight="1">
@@ -2348,7 +2286,7 @@
       <c r="B34" s="59">
         <v>2.1</v>
       </c>
-      <c r="C34" s="72" t="s">
+      <c r="C34" s="65" t="s">
         <v>19</v>
       </c>
       <c r="D34" s="5" t="str">
@@ -2385,13 +2323,13 @@
       <c r="N34" s="10"/>
       <c r="O34" s="10"/>
       <c r="P34" s="10"/>
-      <c r="Q34" s="69"/>
+      <c r="Q34" s="66"/>
       <c r="R34" s="59"/>
     </row>
     <row r="35" spans="1:18" ht="38.25">
       <c r="A35" s="59"/>
       <c r="B35" s="59"/>
-      <c r="C35" s="72"/>
+      <c r="C35" s="65"/>
       <c r="D35" s="5"/>
       <c r="E35" s="9" t="s">
         <v>16</v>
@@ -2423,13 +2361,13 @@
       <c r="N35" s="10"/>
       <c r="O35" s="10"/>
       <c r="P35" s="10"/>
-      <c r="Q35" s="70"/>
+      <c r="Q35" s="67"/>
       <c r="R35" s="59"/>
     </row>
     <row r="36" spans="1:18" ht="38.25">
       <c r="A36" s="59"/>
       <c r="B36" s="59"/>
-      <c r="C36" s="72"/>
+      <c r="C36" s="65"/>
       <c r="D36" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -2464,13 +2402,13 @@
       <c r="N36" s="10"/>
       <c r="O36" s="10"/>
       <c r="P36" s="10"/>
-      <c r="Q36" s="70"/>
+      <c r="Q36" s="67"/>
       <c r="R36" s="59"/>
     </row>
     <row r="37" spans="1:18" ht="15.75">
       <c r="A37" s="59"/>
       <c r="B37" s="59"/>
-      <c r="C37" s="72"/>
+      <c r="C37" s="65"/>
       <c r="D37" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2499,13 +2437,13 @@
       <c r="N37" s="10"/>
       <c r="O37" s="10"/>
       <c r="P37" s="10"/>
-      <c r="Q37" s="70"/>
+      <c r="Q37" s="67"/>
       <c r="R37" s="59"/>
     </row>
     <row r="38" spans="1:18" ht="15.75">
       <c r="A38" s="59"/>
       <c r="B38" s="59"/>
-      <c r="C38" s="72"/>
+      <c r="C38" s="65"/>
       <c r="D38" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2534,13 +2472,13 @@
       <c r="N38" s="10"/>
       <c r="O38" s="10"/>
       <c r="P38" s="10"/>
-      <c r="Q38" s="70"/>
+      <c r="Q38" s="67"/>
       <c r="R38" s="59"/>
     </row>
     <row r="39" spans="1:18" ht="15.75">
       <c r="A39" s="59"/>
       <c r="B39" s="59"/>
-      <c r="C39" s="72"/>
+      <c r="C39" s="65"/>
       <c r="D39" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2569,13 +2507,13 @@
       <c r="N39" s="10"/>
       <c r="O39" s="10"/>
       <c r="P39" s="10"/>
-      <c r="Q39" s="70"/>
+      <c r="Q39" s="67"/>
       <c r="R39" s="59"/>
     </row>
     <row r="40" spans="1:18" ht="15.75">
       <c r="A40" s="59"/>
       <c r="B40" s="59"/>
-      <c r="C40" s="72"/>
+      <c r="C40" s="65"/>
       <c r="D40" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2604,13 +2542,13 @@
       <c r="N40" s="10"/>
       <c r="O40" s="10"/>
       <c r="P40" s="10"/>
-      <c r="Q40" s="70"/>
+      <c r="Q40" s="67"/>
       <c r="R40" s="59"/>
     </row>
     <row r="41" spans="1:18" ht="15.75">
       <c r="A41" s="59"/>
       <c r="B41" s="59"/>
-      <c r="C41" s="72"/>
+      <c r="C41" s="65"/>
       <c r="D41" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2639,13 +2577,13 @@
       <c r="N41" s="10"/>
       <c r="O41" s="10"/>
       <c r="P41" s="10"/>
-      <c r="Q41" s="70"/>
+      <c r="Q41" s="67"/>
       <c r="R41" s="59"/>
     </row>
     <row r="42" spans="1:18" ht="15.75">
       <c r="A42" s="59"/>
       <c r="B42" s="59"/>
-      <c r="C42" s="72"/>
+      <c r="C42" s="65"/>
       <c r="D42" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2674,13 +2612,13 @@
       <c r="N42" s="10"/>
       <c r="O42" s="10"/>
       <c r="P42" s="10"/>
-      <c r="Q42" s="70"/>
+      <c r="Q42" s="67"/>
       <c r="R42" s="59"/>
     </row>
     <row r="43" spans="1:18" ht="15.75">
       <c r="A43" s="59"/>
       <c r="B43" s="59"/>
-      <c r="C43" s="72"/>
+      <c r="C43" s="65"/>
       <c r="D43" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2709,13 +2647,13 @@
       <c r="N43" s="10"/>
       <c r="O43" s="10"/>
       <c r="P43" s="10"/>
-      <c r="Q43" s="70"/>
+      <c r="Q43" s="67"/>
       <c r="R43" s="59"/>
     </row>
     <row r="44" spans="1:18" ht="15.75">
       <c r="A44" s="59"/>
       <c r="B44" s="59"/>
-      <c r="C44" s="72"/>
+      <c r="C44" s="65"/>
       <c r="D44" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2744,13 +2682,13 @@
       <c r="N44" s="10"/>
       <c r="O44" s="10"/>
       <c r="P44" s="10"/>
-      <c r="Q44" s="70"/>
+      <c r="Q44" s="67"/>
       <c r="R44" s="59"/>
     </row>
     <row r="45" spans="1:18" ht="15.75">
       <c r="A45" s="59"/>
       <c r="B45" s="59"/>
-      <c r="C45" s="72"/>
+      <c r="C45" s="65"/>
       <c r="D45" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2779,13 +2717,13 @@
       <c r="N45" s="10"/>
       <c r="O45" s="10"/>
       <c r="P45" s="10"/>
-      <c r="Q45" s="70"/>
+      <c r="Q45" s="67"/>
       <c r="R45" s="59"/>
     </row>
     <row r="46" spans="1:18" ht="15.75">
       <c r="A46" s="59"/>
       <c r="B46" s="59"/>
-      <c r="C46" s="72"/>
+      <c r="C46" s="65"/>
       <c r="D46" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2814,13 +2752,13 @@
       <c r="N46" s="10"/>
       <c r="O46" s="10"/>
       <c r="P46" s="10"/>
-      <c r="Q46" s="70"/>
+      <c r="Q46" s="67"/>
       <c r="R46" s="59"/>
     </row>
     <row r="47" spans="1:18" ht="15.75">
       <c r="A47" s="59"/>
       <c r="B47" s="59"/>
-      <c r="C47" s="72"/>
+      <c r="C47" s="65"/>
       <c r="D47" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2849,13 +2787,13 @@
       <c r="N47" s="10"/>
       <c r="O47" s="10"/>
       <c r="P47" s="10"/>
-      <c r="Q47" s="70"/>
+      <c r="Q47" s="67"/>
       <c r="R47" s="59"/>
     </row>
     <row r="48" spans="1:18" ht="15.75">
       <c r="A48" s="59"/>
       <c r="B48" s="59"/>
-      <c r="C48" s="72"/>
+      <c r="C48" s="65"/>
       <c r="D48" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -2884,7 +2822,7 @@
       <c r="N48" s="10"/>
       <c r="O48" s="10"/>
       <c r="P48" s="10"/>
-      <c r="Q48" s="71"/>
+      <c r="Q48" s="68"/>
       <c r="R48" s="59"/>
     </row>
     <row r="49" spans="1:18" ht="63.75">
@@ -2892,7 +2830,7 @@
       <c r="B49" s="59">
         <v>2.2000000000000002</v>
       </c>
-      <c r="C49" s="72" t="s">
+      <c r="C49" s="65" t="s">
         <v>20</v>
       </c>
       <c r="D49" s="5" t="str">
@@ -2929,13 +2867,13 @@
       <c r="N49" s="10"/>
       <c r="O49" s="10"/>
       <c r="P49" s="10"/>
-      <c r="Q49" s="69"/>
+      <c r="Q49" s="66"/>
       <c r="R49" s="59"/>
     </row>
     <row r="50" spans="1:18" ht="38.25">
       <c r="A50" s="59"/>
       <c r="B50" s="59"/>
-      <c r="C50" s="72"/>
+      <c r="C50" s="65"/>
       <c r="D50" s="5" t="s">
         <v>21</v>
       </c>
@@ -2969,13 +2907,13 @@
       <c r="N50" s="10"/>
       <c r="O50" s="10"/>
       <c r="P50" s="10"/>
-      <c r="Q50" s="70"/>
+      <c r="Q50" s="67"/>
       <c r="R50" s="59"/>
     </row>
     <row r="51" spans="1:18" ht="38.25">
       <c r="A51" s="59"/>
       <c r="B51" s="59"/>
-      <c r="C51" s="72"/>
+      <c r="C51" s="65"/>
       <c r="D51" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -3010,13 +2948,13 @@
       <c r="N51" s="10"/>
       <c r="O51" s="10"/>
       <c r="P51" s="10"/>
-      <c r="Q51" s="70"/>
+      <c r="Q51" s="67"/>
       <c r="R51" s="59"/>
     </row>
     <row r="52" spans="1:18" ht="15.75">
       <c r="A52" s="59"/>
       <c r="B52" s="59"/>
-      <c r="C52" s="72"/>
+      <c r="C52" s="65"/>
       <c r="D52" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3045,13 +2983,13 @@
       <c r="N52" s="10"/>
       <c r="O52" s="10"/>
       <c r="P52" s="10"/>
-      <c r="Q52" s="70"/>
+      <c r="Q52" s="67"/>
       <c r="R52" s="59"/>
     </row>
     <row r="53" spans="1:18" ht="15.75">
       <c r="A53" s="59"/>
       <c r="B53" s="59"/>
-      <c r="C53" s="72"/>
+      <c r="C53" s="65"/>
       <c r="D53" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3080,13 +3018,13 @@
       <c r="N53" s="10"/>
       <c r="O53" s="10"/>
       <c r="P53" s="10"/>
-      <c r="Q53" s="70"/>
+      <c r="Q53" s="67"/>
       <c r="R53" s="59"/>
     </row>
     <row r="54" spans="1:18" ht="15.75">
       <c r="A54" s="59"/>
       <c r="B54" s="59"/>
-      <c r="C54" s="72"/>
+      <c r="C54" s="65"/>
       <c r="D54" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3115,13 +3053,13 @@
       <c r="N54" s="10"/>
       <c r="O54" s="10"/>
       <c r="P54" s="10"/>
-      <c r="Q54" s="70"/>
+      <c r="Q54" s="67"/>
       <c r="R54" s="59"/>
     </row>
     <row r="55" spans="1:18" ht="15.75">
       <c r="A55" s="59"/>
       <c r="B55" s="59"/>
-      <c r="C55" s="72"/>
+      <c r="C55" s="65"/>
       <c r="D55" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3150,13 +3088,13 @@
       <c r="N55" s="10"/>
       <c r="O55" s="10"/>
       <c r="P55" s="10"/>
-      <c r="Q55" s="70"/>
+      <c r="Q55" s="67"/>
       <c r="R55" s="59"/>
     </row>
     <row r="56" spans="1:18" ht="15.75">
       <c r="A56" s="59"/>
       <c r="B56" s="59"/>
-      <c r="C56" s="72"/>
+      <c r="C56" s="65"/>
       <c r="D56" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3185,13 +3123,13 @@
       <c r="N56" s="10"/>
       <c r="O56" s="10"/>
       <c r="P56" s="10"/>
-      <c r="Q56" s="70"/>
+      <c r="Q56" s="67"/>
       <c r="R56" s="59"/>
     </row>
     <row r="57" spans="1:18" ht="15.75">
       <c r="A57" s="59"/>
       <c r="B57" s="59"/>
-      <c r="C57" s="72"/>
+      <c r="C57" s="65"/>
       <c r="D57" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3220,13 +3158,13 @@
       <c r="N57" s="10"/>
       <c r="O57" s="10"/>
       <c r="P57" s="10"/>
-      <c r="Q57" s="70"/>
+      <c r="Q57" s="67"/>
       <c r="R57" s="59"/>
     </row>
     <row r="58" spans="1:18" ht="15.75">
       <c r="A58" s="59"/>
       <c r="B58" s="59"/>
-      <c r="C58" s="72"/>
+      <c r="C58" s="65"/>
       <c r="D58" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3255,13 +3193,13 @@
       <c r="N58" s="10"/>
       <c r="O58" s="10"/>
       <c r="P58" s="10"/>
-      <c r="Q58" s="70"/>
+      <c r="Q58" s="67"/>
       <c r="R58" s="59"/>
     </row>
     <row r="59" spans="1:18" ht="15.75">
       <c r="A59" s="59"/>
       <c r="B59" s="59"/>
-      <c r="C59" s="72"/>
+      <c r="C59" s="65"/>
       <c r="D59" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3290,13 +3228,13 @@
       <c r="N59" s="10"/>
       <c r="O59" s="10"/>
       <c r="P59" s="10"/>
-      <c r="Q59" s="70"/>
+      <c r="Q59" s="67"/>
       <c r="R59" s="59"/>
     </row>
     <row r="60" spans="1:18" ht="15.75">
       <c r="A60" s="59"/>
       <c r="B60" s="59"/>
-      <c r="C60" s="72"/>
+      <c r="C60" s="65"/>
       <c r="D60" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3325,13 +3263,13 @@
       <c r="N60" s="10"/>
       <c r="O60" s="10"/>
       <c r="P60" s="10"/>
-      <c r="Q60" s="70"/>
+      <c r="Q60" s="67"/>
       <c r="R60" s="59"/>
     </row>
     <row r="61" spans="1:18" ht="15.75">
       <c r="A61" s="59"/>
       <c r="B61" s="59"/>
-      <c r="C61" s="72"/>
+      <c r="C61" s="65"/>
       <c r="D61" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3360,13 +3298,13 @@
       <c r="N61" s="10"/>
       <c r="O61" s="10"/>
       <c r="P61" s="10"/>
-      <c r="Q61" s="70"/>
+      <c r="Q61" s="67"/>
       <c r="R61" s="59"/>
     </row>
     <row r="62" spans="1:18" ht="15.75">
       <c r="A62" s="59"/>
       <c r="B62" s="59"/>
-      <c r="C62" s="72"/>
+      <c r="C62" s="65"/>
       <c r="D62" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3395,13 +3333,13 @@
       <c r="N62" s="10"/>
       <c r="O62" s="10"/>
       <c r="P62" s="10"/>
-      <c r="Q62" s="70"/>
+      <c r="Q62" s="67"/>
       <c r="R62" s="59"/>
     </row>
     <row r="63" spans="1:18" ht="15.75">
       <c r="A63" s="59"/>
       <c r="B63" s="59"/>
-      <c r="C63" s="72"/>
+      <c r="C63" s="65"/>
       <c r="D63" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3430,7 +3368,7 @@
       <c r="N63" s="10"/>
       <c r="O63" s="10"/>
       <c r="P63" s="10"/>
-      <c r="Q63" s="71"/>
+      <c r="Q63" s="68"/>
       <c r="R63" s="59"/>
     </row>
     <row r="64" spans="1:18" ht="66.75" customHeight="1">
@@ -3438,7 +3376,7 @@
       <c r="B64" s="59">
         <v>2.2999999999999998</v>
       </c>
-      <c r="C64" s="72" t="s">
+      <c r="C64" s="65" t="s">
         <v>22</v>
       </c>
       <c r="D64" s="5" t="str">
@@ -3475,13 +3413,13 @@
       <c r="N64" s="10"/>
       <c r="O64" s="10"/>
       <c r="P64" s="10"/>
-      <c r="Q64" s="69"/>
+      <c r="Q64" s="66"/>
       <c r="R64" s="59"/>
     </row>
     <row r="65" spans="1:18" ht="25.5">
       <c r="A65" s="59"/>
       <c r="B65" s="59"/>
-      <c r="C65" s="72"/>
+      <c r="C65" s="65"/>
       <c r="D65" s="5" t="str">
         <f t="shared" si="2"/>
         <v>OK</v>
@@ -3516,13 +3454,13 @@
       <c r="N65" s="10"/>
       <c r="O65" s="10"/>
       <c r="P65" s="10"/>
-      <c r="Q65" s="70"/>
+      <c r="Q65" s="67"/>
       <c r="R65" s="59"/>
     </row>
     <row r="66" spans="1:18" ht="15.75">
       <c r="A66" s="59"/>
       <c r="B66" s="59"/>
-      <c r="C66" s="72"/>
+      <c r="C66" s="65"/>
       <c r="D66" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3551,13 +3489,13 @@
       <c r="N66" s="10"/>
       <c r="O66" s="10"/>
       <c r="P66" s="10"/>
-      <c r="Q66" s="70"/>
+      <c r="Q66" s="67"/>
       <c r="R66" s="59"/>
     </row>
     <row r="67" spans="1:18" ht="15.75">
       <c r="A67" s="59"/>
       <c r="B67" s="59"/>
-      <c r="C67" s="72"/>
+      <c r="C67" s="65"/>
       <c r="D67" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3586,13 +3524,13 @@
       <c r="N67" s="10"/>
       <c r="O67" s="10"/>
       <c r="P67" s="10"/>
-      <c r="Q67" s="70"/>
+      <c r="Q67" s="67"/>
       <c r="R67" s="59"/>
     </row>
     <row r="68" spans="1:18" ht="15.75">
       <c r="A68" s="59"/>
       <c r="B68" s="59"/>
-      <c r="C68" s="72"/>
+      <c r="C68" s="65"/>
       <c r="D68" s="5" t="str">
         <f t="shared" si="2"/>
         <v>-</v>
@@ -3621,13 +3559,13 @@
       <c r="N68" s="10"/>
       <c r="O68" s="10"/>
       <c r="P68" s="10"/>
-      <c r="Q68" s="70"/>
+      <c r="Q68" s="67"/>
       <c r="R68" s="59"/>
     </row>
     <row r="69" spans="1:18" ht="15.75">
       <c r="A69" s="59"/>
       <c r="B69" s="59"/>
-      <c r="C69" s="72"/>
+      <c r="C69" s="65"/>
       <c r="D69" s="5" t="str">
         <f t="shared" ref="D69:D132" si="5">IF(LEN(E69)&gt;5,IF(LEN(K69&amp;L69&amp;M69)&gt;=1,"OK","Check"),"-")</f>
         <v>-</v>
@@ -3656,13 +3594,13 @@
       <c r="N69" s="10"/>
       <c r="O69" s="10"/>
       <c r="P69" s="10"/>
-      <c r="Q69" s="70"/>
+      <c r="Q69" s="67"/>
       <c r="R69" s="59"/>
     </row>
     <row r="70" spans="1:18" ht="15.75">
       <c r="A70" s="59"/>
       <c r="B70" s="59"/>
-      <c r="C70" s="72"/>
+      <c r="C70" s="65"/>
       <c r="D70" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3691,13 +3629,13 @@
       <c r="N70" s="10"/>
       <c r="O70" s="10"/>
       <c r="P70" s="10"/>
-      <c r="Q70" s="70"/>
+      <c r="Q70" s="67"/>
       <c r="R70" s="59"/>
     </row>
     <row r="71" spans="1:18" ht="15.75">
       <c r="A71" s="59"/>
       <c r="B71" s="59"/>
-      <c r="C71" s="72"/>
+      <c r="C71" s="65"/>
       <c r="D71" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3726,13 +3664,13 @@
       <c r="N71" s="10"/>
       <c r="O71" s="10"/>
       <c r="P71" s="10"/>
-      <c r="Q71" s="70"/>
+      <c r="Q71" s="67"/>
       <c r="R71" s="59"/>
     </row>
     <row r="72" spans="1:18" ht="15.75">
       <c r="A72" s="59"/>
       <c r="B72" s="59"/>
-      <c r="C72" s="72"/>
+      <c r="C72" s="65"/>
       <c r="D72" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3761,13 +3699,13 @@
       <c r="N72" s="10"/>
       <c r="O72" s="10"/>
       <c r="P72" s="10"/>
-      <c r="Q72" s="70"/>
+      <c r="Q72" s="67"/>
       <c r="R72" s="59"/>
     </row>
     <row r="73" spans="1:18" ht="15.75">
       <c r="A73" s="59"/>
       <c r="B73" s="59"/>
-      <c r="C73" s="72"/>
+      <c r="C73" s="65"/>
       <c r="D73" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3796,13 +3734,13 @@
       <c r="N73" s="10"/>
       <c r="O73" s="10"/>
       <c r="P73" s="10"/>
-      <c r="Q73" s="70"/>
+      <c r="Q73" s="67"/>
       <c r="R73" s="59"/>
     </row>
     <row r="74" spans="1:18" ht="15.75">
       <c r="A74" s="59"/>
       <c r="B74" s="59"/>
-      <c r="C74" s="72"/>
+      <c r="C74" s="65"/>
       <c r="D74" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3831,13 +3769,13 @@
       <c r="N74" s="10"/>
       <c r="O74" s="10"/>
       <c r="P74" s="10"/>
-      <c r="Q74" s="70"/>
+      <c r="Q74" s="67"/>
       <c r="R74" s="59"/>
     </row>
     <row r="75" spans="1:18" ht="15.75">
       <c r="A75" s="59"/>
       <c r="B75" s="59"/>
-      <c r="C75" s="72"/>
+      <c r="C75" s="65"/>
       <c r="D75" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3866,13 +3804,13 @@
       <c r="N75" s="10"/>
       <c r="O75" s="10"/>
       <c r="P75" s="10"/>
-      <c r="Q75" s="70"/>
+      <c r="Q75" s="67"/>
       <c r="R75" s="59"/>
     </row>
     <row r="76" spans="1:18" ht="15.75">
       <c r="A76" s="59"/>
       <c r="B76" s="59"/>
-      <c r="C76" s="72"/>
+      <c r="C76" s="65"/>
       <c r="D76" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3901,13 +3839,13 @@
       <c r="N76" s="10"/>
       <c r="O76" s="10"/>
       <c r="P76" s="10"/>
-      <c r="Q76" s="70"/>
+      <c r="Q76" s="67"/>
       <c r="R76" s="59"/>
     </row>
     <row r="77" spans="1:18" ht="15.75">
       <c r="A77" s="59"/>
       <c r="B77" s="59"/>
-      <c r="C77" s="72"/>
+      <c r="C77" s="65"/>
       <c r="D77" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3936,13 +3874,13 @@
       <c r="N77" s="10"/>
       <c r="O77" s="10"/>
       <c r="P77" s="10"/>
-      <c r="Q77" s="70"/>
+      <c r="Q77" s="67"/>
       <c r="R77" s="59"/>
     </row>
     <row r="78" spans="1:18" ht="15.75">
       <c r="A78" s="59"/>
       <c r="B78" s="59"/>
-      <c r="C78" s="72"/>
+      <c r="C78" s="65"/>
       <c r="D78" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -3971,7 +3909,7 @@
       <c r="N78" s="10"/>
       <c r="O78" s="10"/>
       <c r="P78" s="10"/>
-      <c r="Q78" s="71"/>
+      <c r="Q78" s="68"/>
       <c r="R78" s="59"/>
     </row>
     <row r="79" spans="1:18" ht="38.25">
@@ -3981,7 +3919,7 @@
       <c r="B79" s="59">
         <v>3.1</v>
       </c>
-      <c r="C79" s="72" t="s">
+      <c r="C79" s="65" t="s">
         <v>24</v>
       </c>
       <c r="D79" s="5" t="str">
@@ -4018,13 +3956,13 @@
       <c r="N79" s="10"/>
       <c r="O79" s="10"/>
       <c r="P79" s="10"/>
-      <c r="Q79" s="69"/>
+      <c r="Q79" s="66"/>
       <c r="R79" s="59"/>
     </row>
     <row r="80" spans="1:18" ht="38.25">
       <c r="A80" s="59"/>
       <c r="B80" s="59"/>
-      <c r="C80" s="72"/>
+      <c r="C80" s="65"/>
       <c r="D80" s="5" t="str">
         <f t="shared" si="5"/>
         <v>OK</v>
@@ -4059,13 +3997,13 @@
       <c r="N80" s="10"/>
       <c r="O80" s="10"/>
       <c r="P80" s="10"/>
-      <c r="Q80" s="70"/>
+      <c r="Q80" s="67"/>
       <c r="R80" s="59"/>
     </row>
     <row r="81" spans="1:18" ht="15.75">
       <c r="A81" s="59"/>
       <c r="B81" s="59"/>
-      <c r="C81" s="72"/>
+      <c r="C81" s="65"/>
       <c r="D81" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4094,13 +4032,13 @@
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
       <c r="P81" s="10"/>
-      <c r="Q81" s="70"/>
+      <c r="Q81" s="67"/>
       <c r="R81" s="59"/>
     </row>
     <row r="82" spans="1:18" ht="15.75">
       <c r="A82" s="59"/>
       <c r="B82" s="59"/>
-      <c r="C82" s="72"/>
+      <c r="C82" s="65"/>
       <c r="D82" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4129,13 +4067,13 @@
       <c r="N82" s="10"/>
       <c r="O82" s="10"/>
       <c r="P82" s="10"/>
-      <c r="Q82" s="70"/>
+      <c r="Q82" s="67"/>
       <c r="R82" s="59"/>
     </row>
     <row r="83" spans="1:18" ht="15.75">
       <c r="A83" s="59"/>
       <c r="B83" s="59"/>
-      <c r="C83" s="72"/>
+      <c r="C83" s="65"/>
       <c r="D83" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4164,13 +4102,13 @@
       <c r="N83" s="10"/>
       <c r="O83" s="10"/>
       <c r="P83" s="10"/>
-      <c r="Q83" s="70"/>
+      <c r="Q83" s="67"/>
       <c r="R83" s="59"/>
     </row>
     <row r="84" spans="1:18" ht="15.75">
       <c r="A84" s="59"/>
       <c r="B84" s="59"/>
-      <c r="C84" s="72"/>
+      <c r="C84" s="65"/>
       <c r="D84" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4199,13 +4137,13 @@
       <c r="N84" s="10"/>
       <c r="O84" s="10"/>
       <c r="P84" s="10"/>
-      <c r="Q84" s="70"/>
+      <c r="Q84" s="67"/>
       <c r="R84" s="59"/>
     </row>
     <row r="85" spans="1:18" ht="15.75">
       <c r="A85" s="59"/>
       <c r="B85" s="59"/>
-      <c r="C85" s="72"/>
+      <c r="C85" s="65"/>
       <c r="D85" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4234,13 +4172,13 @@
       <c r="N85" s="10"/>
       <c r="O85" s="10"/>
       <c r="P85" s="10"/>
-      <c r="Q85" s="70"/>
+      <c r="Q85" s="67"/>
       <c r="R85" s="59"/>
     </row>
     <row r="86" spans="1:18" ht="15.75">
       <c r="A86" s="59"/>
       <c r="B86" s="59"/>
-      <c r="C86" s="72"/>
+      <c r="C86" s="65"/>
       <c r="D86" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4269,13 +4207,13 @@
       <c r="N86" s="10"/>
       <c r="O86" s="10"/>
       <c r="P86" s="10"/>
-      <c r="Q86" s="70"/>
+      <c r="Q86" s="67"/>
       <c r="R86" s="59"/>
     </row>
     <row r="87" spans="1:18" ht="15.75">
       <c r="A87" s="59"/>
       <c r="B87" s="59"/>
-      <c r="C87" s="72"/>
+      <c r="C87" s="65"/>
       <c r="D87" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4304,13 +4242,13 @@
       <c r="N87" s="10"/>
       <c r="O87" s="10"/>
       <c r="P87" s="10"/>
-      <c r="Q87" s="70"/>
+      <c r="Q87" s="67"/>
       <c r="R87" s="59"/>
     </row>
     <row r="88" spans="1:18" ht="15.75">
       <c r="A88" s="59"/>
       <c r="B88" s="59"/>
-      <c r="C88" s="72"/>
+      <c r="C88" s="65"/>
       <c r="D88" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4339,13 +4277,13 @@
       <c r="N88" s="10"/>
       <c r="O88" s="10"/>
       <c r="P88" s="10"/>
-      <c r="Q88" s="70"/>
+      <c r="Q88" s="67"/>
       <c r="R88" s="59"/>
     </row>
     <row r="89" spans="1:18" ht="15.75">
       <c r="A89" s="59"/>
       <c r="B89" s="59"/>
-      <c r="C89" s="72"/>
+      <c r="C89" s="65"/>
       <c r="D89" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4374,13 +4312,13 @@
       <c r="N89" s="10"/>
       <c r="O89" s="10"/>
       <c r="P89" s="10"/>
-      <c r="Q89" s="70"/>
+      <c r="Q89" s="67"/>
       <c r="R89" s="59"/>
     </row>
     <row r="90" spans="1:18" ht="15.75">
       <c r="A90" s="59"/>
       <c r="B90" s="59"/>
-      <c r="C90" s="72"/>
+      <c r="C90" s="65"/>
       <c r="D90" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4409,13 +4347,13 @@
       <c r="N90" s="10"/>
       <c r="O90" s="10"/>
       <c r="P90" s="10"/>
-      <c r="Q90" s="70"/>
+      <c r="Q90" s="67"/>
       <c r="R90" s="59"/>
     </row>
     <row r="91" spans="1:18" ht="15.75">
       <c r="A91" s="59"/>
       <c r="B91" s="59"/>
-      <c r="C91" s="72"/>
+      <c r="C91" s="65"/>
       <c r="D91" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4444,13 +4382,13 @@
       <c r="N91" s="10"/>
       <c r="O91" s="10"/>
       <c r="P91" s="10"/>
-      <c r="Q91" s="70"/>
+      <c r="Q91" s="67"/>
       <c r="R91" s="59"/>
     </row>
     <row r="92" spans="1:18" ht="15.75">
       <c r="A92" s="59"/>
       <c r="B92" s="59"/>
-      <c r="C92" s="72"/>
+      <c r="C92" s="65"/>
       <c r="D92" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4479,13 +4417,13 @@
       <c r="N92" s="10"/>
       <c r="O92" s="10"/>
       <c r="P92" s="10"/>
-      <c r="Q92" s="70"/>
+      <c r="Q92" s="67"/>
       <c r="R92" s="59"/>
     </row>
     <row r="93" spans="1:18" ht="15.75">
       <c r="A93" s="59"/>
       <c r="B93" s="59"/>
-      <c r="C93" s="72"/>
+      <c r="C93" s="65"/>
       <c r="D93" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4514,7 +4452,7 @@
       <c r="N93" s="10"/>
       <c r="O93" s="10"/>
       <c r="P93" s="10"/>
-      <c r="Q93" s="71"/>
+      <c r="Q93" s="68"/>
       <c r="R93" s="59"/>
     </row>
     <row r="94" spans="1:18" ht="38.25">
@@ -4522,7 +4460,7 @@
       <c r="B94" s="60">
         <v>3.2</v>
       </c>
-      <c r="C94" s="72" t="s">
+      <c r="C94" s="65" t="s">
         <v>25</v>
       </c>
       <c r="D94" s="5" t="str">
@@ -4559,18 +4497,20 @@
       <c r="N94" s="10"/>
       <c r="O94" s="10"/>
       <c r="P94" s="10"/>
-      <c r="Q94" s="65"/>
+      <c r="Q94" s="61"/>
       <c r="R94" s="60"/>
     </row>
-    <row r="95" spans="1:18" ht="15.75">
+    <row r="95" spans="1:18" ht="25.5">
       <c r="A95" s="59"/>
       <c r="B95" s="60"/>
-      <c r="C95" s="72"/>
+      <c r="C95" s="65"/>
       <c r="D95" s="5" t="str">
         <f t="shared" si="5"/>
-        <v>-</v>
-      </c>
-      <c r="E95" s="73"/>
+        <v>OK</v>
+      </c>
+      <c r="E95" s="8" t="s">
+        <v>51</v>
+      </c>
       <c r="F95" s="13" t="s">
         <v>50</v>
       </c>
@@ -4585,26 +4525,26 @@
       <c r="J95" s="12"/>
       <c r="K95" s="7" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="L95" s="7" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="M95" s="7" t="str">
         <f t="shared" si="7"/>
-        <v/>
+        <v>X</v>
       </c>
       <c r="N95" s="10"/>
       <c r="O95" s="10"/>
       <c r="P95" s="10"/>
-      <c r="Q95" s="66"/>
+      <c r="Q95" s="62"/>
       <c r="R95" s="60"/>
     </row>
     <row r="96" spans="1:18" ht="28.5" customHeight="1">
       <c r="A96" s="59"/>
       <c r="B96" s="60"/>
-      <c r="C96" s="72"/>
+      <c r="C96" s="65"/>
       <c r="D96" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4633,13 +4573,13 @@
       <c r="N96" s="10"/>
       <c r="O96" s="10"/>
       <c r="P96" s="10"/>
-      <c r="Q96" s="66"/>
+      <c r="Q96" s="62"/>
       <c r="R96" s="60"/>
     </row>
     <row r="97" spans="1:18" ht="15.75">
       <c r="A97" s="59"/>
       <c r="B97" s="60"/>
-      <c r="C97" s="72"/>
+      <c r="C97" s="65"/>
       <c r="D97" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4668,13 +4608,13 @@
       <c r="N97" s="10"/>
       <c r="O97" s="10"/>
       <c r="P97" s="10"/>
-      <c r="Q97" s="66"/>
+      <c r="Q97" s="62"/>
       <c r="R97" s="60"/>
     </row>
     <row r="98" spans="1:18" ht="15.75">
       <c r="A98" s="59"/>
       <c r="B98" s="60"/>
-      <c r="C98" s="72"/>
+      <c r="C98" s="65"/>
       <c r="D98" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4703,13 +4643,13 @@
       <c r="N98" s="10"/>
       <c r="O98" s="10"/>
       <c r="P98" s="10"/>
-      <c r="Q98" s="66"/>
+      <c r="Q98" s="62"/>
       <c r="R98" s="60"/>
     </row>
     <row r="99" spans="1:18" ht="15.75">
       <c r="A99" s="59"/>
       <c r="B99" s="60"/>
-      <c r="C99" s="72"/>
+      <c r="C99" s="65"/>
       <c r="D99" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4738,13 +4678,13 @@
       <c r="N99" s="10"/>
       <c r="O99" s="10"/>
       <c r="P99" s="10"/>
-      <c r="Q99" s="66"/>
+      <c r="Q99" s="62"/>
       <c r="R99" s="60"/>
     </row>
     <row r="100" spans="1:18" ht="15.75">
       <c r="A100" s="59"/>
       <c r="B100" s="60"/>
-      <c r="C100" s="72"/>
+      <c r="C100" s="65"/>
       <c r="D100" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4773,13 +4713,13 @@
       <c r="N100" s="10"/>
       <c r="O100" s="10"/>
       <c r="P100" s="10"/>
-      <c r="Q100" s="66"/>
+      <c r="Q100" s="62"/>
       <c r="R100" s="60"/>
     </row>
     <row r="101" spans="1:18" ht="15.75">
       <c r="A101" s="59"/>
       <c r="B101" s="60"/>
-      <c r="C101" s="72"/>
+      <c r="C101" s="65"/>
       <c r="D101" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4808,13 +4748,13 @@
       <c r="N101" s="10"/>
       <c r="O101" s="10"/>
       <c r="P101" s="10"/>
-      <c r="Q101" s="66"/>
+      <c r="Q101" s="62"/>
       <c r="R101" s="60"/>
     </row>
     <row r="102" spans="1:18" ht="15.75">
       <c r="A102" s="59"/>
       <c r="B102" s="60"/>
-      <c r="C102" s="72"/>
+      <c r="C102" s="65"/>
       <c r="D102" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4843,13 +4783,13 @@
       <c r="N102" s="10"/>
       <c r="O102" s="10"/>
       <c r="P102" s="10"/>
-      <c r="Q102" s="66"/>
+      <c r="Q102" s="62"/>
       <c r="R102" s="60"/>
     </row>
     <row r="103" spans="1:18" ht="15.75">
       <c r="A103" s="59"/>
       <c r="B103" s="60"/>
-      <c r="C103" s="72"/>
+      <c r="C103" s="65"/>
       <c r="D103" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4878,13 +4818,13 @@
       <c r="N103" s="10"/>
       <c r="O103" s="10"/>
       <c r="P103" s="10"/>
-      <c r="Q103" s="66"/>
+      <c r="Q103" s="62"/>
       <c r="R103" s="60"/>
     </row>
     <row r="104" spans="1:18" ht="15.75">
       <c r="A104" s="59"/>
       <c r="B104" s="60"/>
-      <c r="C104" s="72"/>
+      <c r="C104" s="65"/>
       <c r="D104" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4913,13 +4853,13 @@
       <c r="N104" s="10"/>
       <c r="O104" s="10"/>
       <c r="P104" s="10"/>
-      <c r="Q104" s="66"/>
+      <c r="Q104" s="62"/>
       <c r="R104" s="60"/>
     </row>
     <row r="105" spans="1:18" ht="15.75">
       <c r="A105" s="59"/>
       <c r="B105" s="60"/>
-      <c r="C105" s="72"/>
+      <c r="C105" s="65"/>
       <c r="D105" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4948,13 +4888,13 @@
       <c r="N105" s="10"/>
       <c r="O105" s="10"/>
       <c r="P105" s="10"/>
-      <c r="Q105" s="66"/>
+      <c r="Q105" s="62"/>
       <c r="R105" s="60"/>
     </row>
     <row r="106" spans="1:18" ht="15.75">
       <c r="A106" s="59"/>
       <c r="B106" s="60"/>
-      <c r="C106" s="72"/>
+      <c r="C106" s="65"/>
       <c r="D106" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -4983,13 +4923,13 @@
       <c r="N106" s="10"/>
       <c r="O106" s="10"/>
       <c r="P106" s="10"/>
-      <c r="Q106" s="66"/>
+      <c r="Q106" s="62"/>
       <c r="R106" s="60"/>
     </row>
     <row r="107" spans="1:18" ht="15.75">
       <c r="A107" s="59"/>
       <c r="B107" s="60"/>
-      <c r="C107" s="72"/>
+      <c r="C107" s="65"/>
       <c r="D107" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5018,13 +4958,13 @@
       <c r="N107" s="10"/>
       <c r="O107" s="10"/>
       <c r="P107" s="10"/>
-      <c r="Q107" s="66"/>
+      <c r="Q107" s="62"/>
       <c r="R107" s="60"/>
     </row>
     <row r="108" spans="1:18" ht="15.75">
       <c r="A108" s="59"/>
       <c r="B108" s="60"/>
-      <c r="C108" s="72"/>
+      <c r="C108" s="65"/>
       <c r="D108" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5053,13 +4993,13 @@
       <c r="N108" s="10"/>
       <c r="O108" s="10"/>
       <c r="P108" s="10"/>
-      <c r="Q108" s="67"/>
+      <c r="Q108" s="63"/>
       <c r="R108" s="60"/>
     </row>
     <row r="109" spans="1:18" ht="15.75">
       <c r="A109" s="16"/>
       <c r="B109" s="60"/>
-      <c r="C109" s="72"/>
+      <c r="C109" s="65"/>
       <c r="D109" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5088,13 +5028,13 @@
       <c r="N109" s="10"/>
       <c r="O109" s="10"/>
       <c r="P109" s="10"/>
-      <c r="Q109" s="65"/>
+      <c r="Q109" s="61"/>
       <c r="R109" s="60"/>
     </row>
     <row r="110" spans="1:18" ht="15.75">
       <c r="A110" s="16"/>
       <c r="B110" s="60"/>
-      <c r="C110" s="72"/>
+      <c r="C110" s="65"/>
       <c r="D110" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5123,13 +5063,13 @@
       <c r="N110" s="10"/>
       <c r="O110" s="10"/>
       <c r="P110" s="10"/>
-      <c r="Q110" s="66"/>
+      <c r="Q110" s="62"/>
       <c r="R110" s="60"/>
     </row>
     <row r="111" spans="1:18" ht="15.75">
       <c r="A111" s="16"/>
       <c r="B111" s="60"/>
-      <c r="C111" s="72"/>
+      <c r="C111" s="65"/>
       <c r="D111" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5158,13 +5098,13 @@
       <c r="N111" s="10"/>
       <c r="O111" s="10"/>
       <c r="P111" s="10"/>
-      <c r="Q111" s="66"/>
+      <c r="Q111" s="62"/>
       <c r="R111" s="60"/>
     </row>
     <row r="112" spans="1:18" ht="15.75">
       <c r="A112" s="16"/>
       <c r="B112" s="60"/>
-      <c r="C112" s="72"/>
+      <c r="C112" s="65"/>
       <c r="D112" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5193,13 +5133,13 @@
       <c r="N112" s="10"/>
       <c r="O112" s="10"/>
       <c r="P112" s="10"/>
-      <c r="Q112" s="66"/>
+      <c r="Q112" s="62"/>
       <c r="R112" s="60"/>
     </row>
     <row r="113" spans="1:18" ht="15.75">
       <c r="A113" s="16"/>
       <c r="B113" s="60"/>
-      <c r="C113" s="72"/>
+      <c r="C113" s="65"/>
       <c r="D113" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5228,13 +5168,13 @@
       <c r="N113" s="10"/>
       <c r="O113" s="10"/>
       <c r="P113" s="10"/>
-      <c r="Q113" s="66"/>
+      <c r="Q113" s="62"/>
       <c r="R113" s="60"/>
     </row>
     <row r="114" spans="1:18" ht="15.75">
       <c r="A114" s="16"/>
       <c r="B114" s="60"/>
-      <c r="C114" s="72"/>
+      <c r="C114" s="65"/>
       <c r="D114" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5263,13 +5203,13 @@
       <c r="N114" s="10"/>
       <c r="O114" s="10"/>
       <c r="P114" s="10"/>
-      <c r="Q114" s="66"/>
+      <c r="Q114" s="62"/>
       <c r="R114" s="60"/>
     </row>
     <row r="115" spans="1:18" ht="15.75">
       <c r="A115" s="16"/>
       <c r="B115" s="60"/>
-      <c r="C115" s="72"/>
+      <c r="C115" s="65"/>
       <c r="D115" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5298,13 +5238,13 @@
       <c r="N115" s="10"/>
       <c r="O115" s="10"/>
       <c r="P115" s="10"/>
-      <c r="Q115" s="66"/>
+      <c r="Q115" s="62"/>
       <c r="R115" s="60"/>
     </row>
     <row r="116" spans="1:18" ht="15.75">
       <c r="A116" s="16"/>
       <c r="B116" s="60"/>
-      <c r="C116" s="72"/>
+      <c r="C116" s="65"/>
       <c r="D116" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5333,13 +5273,13 @@
       <c r="N116" s="10"/>
       <c r="O116" s="10"/>
       <c r="P116" s="10"/>
-      <c r="Q116" s="66"/>
+      <c r="Q116" s="62"/>
       <c r="R116" s="60"/>
     </row>
     <row r="117" spans="1:18" ht="15.75">
       <c r="A117" s="16"/>
       <c r="B117" s="60"/>
-      <c r="C117" s="72"/>
+      <c r="C117" s="65"/>
       <c r="D117" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5368,13 +5308,13 @@
       <c r="N117" s="10"/>
       <c r="O117" s="10"/>
       <c r="P117" s="10"/>
-      <c r="Q117" s="66"/>
+      <c r="Q117" s="62"/>
       <c r="R117" s="60"/>
     </row>
     <row r="118" spans="1:18" ht="15.75">
       <c r="A118" s="16"/>
       <c r="B118" s="60"/>
-      <c r="C118" s="72"/>
+      <c r="C118" s="65"/>
       <c r="D118" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5403,13 +5343,13 @@
       <c r="N118" s="10"/>
       <c r="O118" s="10"/>
       <c r="P118" s="10"/>
-      <c r="Q118" s="66"/>
+      <c r="Q118" s="62"/>
       <c r="R118" s="60"/>
     </row>
     <row r="119" spans="1:18" ht="15.75">
       <c r="A119" s="16"/>
       <c r="B119" s="60"/>
-      <c r="C119" s="72"/>
+      <c r="C119" s="65"/>
       <c r="D119" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5438,13 +5378,13 @@
       <c r="N119" s="10"/>
       <c r="O119" s="10"/>
       <c r="P119" s="10"/>
-      <c r="Q119" s="66"/>
+      <c r="Q119" s="62"/>
       <c r="R119" s="60"/>
     </row>
     <row r="120" spans="1:18" ht="15.75">
       <c r="A120" s="16"/>
       <c r="B120" s="60"/>
-      <c r="C120" s="72"/>
+      <c r="C120" s="65"/>
       <c r="D120" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5473,13 +5413,13 @@
       <c r="N120" s="10"/>
       <c r="O120" s="10"/>
       <c r="P120" s="10"/>
-      <c r="Q120" s="66"/>
+      <c r="Q120" s="62"/>
       <c r="R120" s="60"/>
     </row>
     <row r="121" spans="1:18" ht="15.75">
       <c r="A121" s="16"/>
       <c r="B121" s="60"/>
-      <c r="C121" s="72"/>
+      <c r="C121" s="65"/>
       <c r="D121" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5508,13 +5448,13 @@
       <c r="N121" s="10"/>
       <c r="O121" s="10"/>
       <c r="P121" s="10"/>
-      <c r="Q121" s="66"/>
+      <c r="Q121" s="62"/>
       <c r="R121" s="60"/>
     </row>
     <row r="122" spans="1:18" ht="15.75">
       <c r="A122" s="16"/>
       <c r="B122" s="60"/>
-      <c r="C122" s="72"/>
+      <c r="C122" s="65"/>
       <c r="D122" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5543,13 +5483,13 @@
       <c r="N122" s="10"/>
       <c r="O122" s="10"/>
       <c r="P122" s="10"/>
-      <c r="Q122" s="66"/>
+      <c r="Q122" s="62"/>
       <c r="R122" s="60"/>
     </row>
     <row r="123" spans="1:18" ht="15.75">
       <c r="A123" s="16"/>
       <c r="B123" s="60"/>
-      <c r="C123" s="72"/>
+      <c r="C123" s="65"/>
       <c r="D123" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5578,13 +5518,13 @@
       <c r="N123" s="10"/>
       <c r="O123" s="10"/>
       <c r="P123" s="10"/>
-      <c r="Q123" s="67"/>
+      <c r="Q123" s="63"/>
       <c r="R123" s="60"/>
     </row>
     <row r="124" spans="1:18" ht="25.5" customHeight="1">
       <c r="A124" s="16"/>
       <c r="B124" s="60"/>
-      <c r="C124" s="72"/>
+      <c r="C124" s="65"/>
       <c r="D124" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5613,13 +5553,13 @@
       <c r="N124" s="10"/>
       <c r="O124" s="10"/>
       <c r="P124" s="10"/>
-      <c r="Q124" s="65"/>
+      <c r="Q124" s="61"/>
       <c r="R124" s="60"/>
     </row>
     <row r="125" spans="1:18" ht="15.75">
       <c r="A125" s="16"/>
       <c r="B125" s="60"/>
-      <c r="C125" s="72"/>
+      <c r="C125" s="65"/>
       <c r="D125" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5648,13 +5588,13 @@
       <c r="N125" s="10"/>
       <c r="O125" s="10"/>
       <c r="P125" s="10"/>
-      <c r="Q125" s="66"/>
+      <c r="Q125" s="62"/>
       <c r="R125" s="60"/>
     </row>
     <row r="126" spans="1:18" ht="15.75">
       <c r="A126" s="16"/>
       <c r="B126" s="60"/>
-      <c r="C126" s="72"/>
+      <c r="C126" s="65"/>
       <c r="D126" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5683,13 +5623,13 @@
       <c r="N126" s="10"/>
       <c r="O126" s="10"/>
       <c r="P126" s="10"/>
-      <c r="Q126" s="66"/>
+      <c r="Q126" s="62"/>
       <c r="R126" s="60"/>
     </row>
     <row r="127" spans="1:18" ht="15.75">
       <c r="A127" s="16"/>
       <c r="B127" s="60"/>
-      <c r="C127" s="72"/>
+      <c r="C127" s="65"/>
       <c r="D127" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5718,13 +5658,13 @@
       <c r="N127" s="10"/>
       <c r="O127" s="10"/>
       <c r="P127" s="10"/>
-      <c r="Q127" s="66"/>
+      <c r="Q127" s="62"/>
       <c r="R127" s="60"/>
     </row>
     <row r="128" spans="1:18" ht="15.75">
       <c r="A128" s="16"/>
       <c r="B128" s="60"/>
-      <c r="C128" s="72"/>
+      <c r="C128" s="65"/>
       <c r="D128" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5753,13 +5693,13 @@
       <c r="N128" s="10"/>
       <c r="O128" s="10"/>
       <c r="P128" s="10"/>
-      <c r="Q128" s="66"/>
+      <c r="Q128" s="62"/>
       <c r="R128" s="60"/>
     </row>
     <row r="129" spans="1:18" ht="15.75">
       <c r="A129" s="16"/>
       <c r="B129" s="60"/>
-      <c r="C129" s="72"/>
+      <c r="C129" s="65"/>
       <c r="D129" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5788,13 +5728,13 @@
       <c r="N129" s="10"/>
       <c r="O129" s="10"/>
       <c r="P129" s="10"/>
-      <c r="Q129" s="66"/>
+      <c r="Q129" s="62"/>
       <c r="R129" s="60"/>
     </row>
     <row r="130" spans="1:18" ht="15.75">
       <c r="A130" s="16"/>
       <c r="B130" s="60"/>
-      <c r="C130" s="72"/>
+      <c r="C130" s="65"/>
       <c r="D130" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5823,13 +5763,13 @@
       <c r="N130" s="10"/>
       <c r="O130" s="10"/>
       <c r="P130" s="10"/>
-      <c r="Q130" s="66"/>
+      <c r="Q130" s="62"/>
       <c r="R130" s="60"/>
     </row>
     <row r="131" spans="1:18" ht="15.75">
       <c r="A131" s="16"/>
       <c r="B131" s="60"/>
-      <c r="C131" s="72"/>
+      <c r="C131" s="65"/>
       <c r="D131" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5858,13 +5798,13 @@
       <c r="N131" s="10"/>
       <c r="O131" s="10"/>
       <c r="P131" s="10"/>
-      <c r="Q131" s="66"/>
+      <c r="Q131" s="62"/>
       <c r="R131" s="60"/>
     </row>
     <row r="132" spans="1:18" ht="15.75">
       <c r="A132" s="16"/>
       <c r="B132" s="60"/>
-      <c r="C132" s="72"/>
+      <c r="C132" s="65"/>
       <c r="D132" s="5" t="str">
         <f t="shared" si="5"/>
         <v>-</v>
@@ -5893,13 +5833,13 @@
       <c r="N132" s="10"/>
       <c r="O132" s="10"/>
       <c r="P132" s="10"/>
-      <c r="Q132" s="66"/>
+      <c r="Q132" s="62"/>
       <c r="R132" s="60"/>
     </row>
     <row r="133" spans="1:18" ht="15.75">
       <c r="A133" s="16"/>
       <c r="B133" s="60"/>
-      <c r="C133" s="72"/>
+      <c r="C133" s="65"/>
       <c r="D133" s="5" t="str">
         <f t="shared" ref="D133:D196" si="8">IF(LEN(E133)&gt;5,IF(LEN(K133&amp;L133&amp;M133)&gt;=1,"OK","Check"),"-")</f>
         <v>-</v>
@@ -5928,13 +5868,13 @@
       <c r="N133" s="10"/>
       <c r="O133" s="10"/>
       <c r="P133" s="10"/>
-      <c r="Q133" s="66"/>
+      <c r="Q133" s="62"/>
       <c r="R133" s="60"/>
     </row>
     <row r="134" spans="1:18" ht="15.75">
       <c r="A134" s="16"/>
       <c r="B134" s="60"/>
-      <c r="C134" s="72"/>
+      <c r="C134" s="65"/>
       <c r="D134" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -5963,13 +5903,13 @@
       <c r="N134" s="10"/>
       <c r="O134" s="10"/>
       <c r="P134" s="10"/>
-      <c r="Q134" s="66"/>
+      <c r="Q134" s="62"/>
       <c r="R134" s="60"/>
     </row>
     <row r="135" spans="1:18" ht="15.75">
       <c r="A135" s="16"/>
       <c r="B135" s="60"/>
-      <c r="C135" s="72"/>
+      <c r="C135" s="65"/>
       <c r="D135" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -5998,13 +5938,13 @@
       <c r="N135" s="10"/>
       <c r="O135" s="10"/>
       <c r="P135" s="10"/>
-      <c r="Q135" s="66"/>
+      <c r="Q135" s="62"/>
       <c r="R135" s="60"/>
     </row>
     <row r="136" spans="1:18" ht="15.75">
       <c r="A136" s="16"/>
       <c r="B136" s="60"/>
-      <c r="C136" s="72"/>
+      <c r="C136" s="65"/>
       <c r="D136" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6033,13 +5973,13 @@
       <c r="N136" s="10"/>
       <c r="O136" s="10"/>
       <c r="P136" s="10"/>
-      <c r="Q136" s="66"/>
+      <c r="Q136" s="62"/>
       <c r="R136" s="60"/>
     </row>
     <row r="137" spans="1:18" ht="15.75">
       <c r="A137" s="16"/>
       <c r="B137" s="60"/>
-      <c r="C137" s="72"/>
+      <c r="C137" s="65"/>
       <c r="D137" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6068,13 +6008,13 @@
       <c r="N137" s="10"/>
       <c r="O137" s="10"/>
       <c r="P137" s="10"/>
-      <c r="Q137" s="66"/>
+      <c r="Q137" s="62"/>
       <c r="R137" s="60"/>
     </row>
     <row r="138" spans="1:18" ht="15.75">
       <c r="A138" s="16"/>
       <c r="B138" s="60"/>
-      <c r="C138" s="72"/>
+      <c r="C138" s="65"/>
       <c r="D138" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6103,13 +6043,13 @@
       <c r="N138" s="10"/>
       <c r="O138" s="10"/>
       <c r="P138" s="10"/>
-      <c r="Q138" s="67"/>
+      <c r="Q138" s="63"/>
       <c r="R138" s="60"/>
     </row>
     <row r="139" spans="1:18" ht="12.75" customHeight="1">
       <c r="A139" s="16"/>
       <c r="B139" s="60"/>
-      <c r="C139" s="72"/>
+      <c r="C139" s="65"/>
       <c r="D139" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6138,13 +6078,13 @@
       <c r="N139" s="10"/>
       <c r="O139" s="10"/>
       <c r="P139" s="10"/>
-      <c r="Q139" s="65"/>
+      <c r="Q139" s="61"/>
       <c r="R139" s="60"/>
     </row>
     <row r="140" spans="1:18" ht="15.75">
       <c r="A140" s="16"/>
       <c r="B140" s="60"/>
-      <c r="C140" s="72"/>
+      <c r="C140" s="65"/>
       <c r="D140" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6173,13 +6113,13 @@
       <c r="N140" s="10"/>
       <c r="O140" s="10"/>
       <c r="P140" s="10"/>
-      <c r="Q140" s="66"/>
+      <c r="Q140" s="62"/>
       <c r="R140" s="60"/>
     </row>
     <row r="141" spans="1:18" ht="15.75">
       <c r="A141" s="16"/>
       <c r="B141" s="60"/>
-      <c r="C141" s="72"/>
+      <c r="C141" s="65"/>
       <c r="D141" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6208,13 +6148,13 @@
       <c r="N141" s="10"/>
       <c r="O141" s="10"/>
       <c r="P141" s="10"/>
-      <c r="Q141" s="66"/>
+      <c r="Q141" s="62"/>
       <c r="R141" s="60"/>
     </row>
     <row r="142" spans="1:18" ht="15.75">
       <c r="A142" s="16"/>
       <c r="B142" s="60"/>
-      <c r="C142" s="72"/>
+      <c r="C142" s="65"/>
       <c r="D142" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6243,13 +6183,13 @@
       <c r="N142" s="10"/>
       <c r="O142" s="10"/>
       <c r="P142" s="10"/>
-      <c r="Q142" s="66"/>
+      <c r="Q142" s="62"/>
       <c r="R142" s="60"/>
     </row>
     <row r="143" spans="1:18" ht="15.75">
       <c r="A143" s="16"/>
       <c r="B143" s="60"/>
-      <c r="C143" s="72"/>
+      <c r="C143" s="65"/>
       <c r="D143" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6278,13 +6218,13 @@
       <c r="N143" s="10"/>
       <c r="O143" s="10"/>
       <c r="P143" s="10"/>
-      <c r="Q143" s="66"/>
+      <c r="Q143" s="62"/>
       <c r="R143" s="60"/>
     </row>
     <row r="144" spans="1:18" ht="15.75">
       <c r="A144" s="16"/>
       <c r="B144" s="60"/>
-      <c r="C144" s="72"/>
+      <c r="C144" s="65"/>
       <c r="D144" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6313,13 +6253,13 @@
       <c r="N144" s="10"/>
       <c r="O144" s="10"/>
       <c r="P144" s="10"/>
-      <c r="Q144" s="66"/>
+      <c r="Q144" s="62"/>
       <c r="R144" s="60"/>
     </row>
     <row r="145" spans="1:18" ht="15.75">
       <c r="A145" s="16"/>
       <c r="B145" s="60"/>
-      <c r="C145" s="72"/>
+      <c r="C145" s="65"/>
       <c r="D145" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6348,13 +6288,13 @@
       <c r="N145" s="10"/>
       <c r="O145" s="10"/>
       <c r="P145" s="10"/>
-      <c r="Q145" s="66"/>
+      <c r="Q145" s="62"/>
       <c r="R145" s="60"/>
     </row>
     <row r="146" spans="1:18" ht="15.75">
       <c r="A146" s="16"/>
       <c r="B146" s="60"/>
-      <c r="C146" s="72"/>
+      <c r="C146" s="65"/>
       <c r="D146" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6383,13 +6323,13 @@
       <c r="N146" s="10"/>
       <c r="O146" s="10"/>
       <c r="P146" s="10"/>
-      <c r="Q146" s="66"/>
+      <c r="Q146" s="62"/>
       <c r="R146" s="60"/>
     </row>
     <row r="147" spans="1:18" ht="15.75">
       <c r="A147" s="16"/>
       <c r="B147" s="60"/>
-      <c r="C147" s="72"/>
+      <c r="C147" s="65"/>
       <c r="D147" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6418,13 +6358,13 @@
       <c r="N147" s="10"/>
       <c r="O147" s="10"/>
       <c r="P147" s="10"/>
-      <c r="Q147" s="66"/>
+      <c r="Q147" s="62"/>
       <c r="R147" s="60"/>
     </row>
     <row r="148" spans="1:18" ht="15.75">
       <c r="A148" s="16"/>
       <c r="B148" s="60"/>
-      <c r="C148" s="72"/>
+      <c r="C148" s="65"/>
       <c r="D148" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6453,13 +6393,13 @@
       <c r="N148" s="10"/>
       <c r="O148" s="10"/>
       <c r="P148" s="10"/>
-      <c r="Q148" s="66"/>
+      <c r="Q148" s="62"/>
       <c r="R148" s="60"/>
     </row>
     <row r="149" spans="1:18" ht="15.75">
       <c r="A149" s="16"/>
       <c r="B149" s="60"/>
-      <c r="C149" s="72"/>
+      <c r="C149" s="65"/>
       <c r="D149" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6488,13 +6428,13 @@
       <c r="N149" s="10"/>
       <c r="O149" s="10"/>
       <c r="P149" s="10"/>
-      <c r="Q149" s="66"/>
+      <c r="Q149" s="62"/>
       <c r="R149" s="60"/>
     </row>
     <row r="150" spans="1:18" ht="15.75">
       <c r="A150" s="16"/>
       <c r="B150" s="60"/>
-      <c r="C150" s="72"/>
+      <c r="C150" s="65"/>
       <c r="D150" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6523,13 +6463,13 @@
       <c r="N150" s="10"/>
       <c r="O150" s="10"/>
       <c r="P150" s="10"/>
-      <c r="Q150" s="66"/>
+      <c r="Q150" s="62"/>
       <c r="R150" s="60"/>
     </row>
     <row r="151" spans="1:18" ht="15.75">
       <c r="A151" s="16"/>
       <c r="B151" s="60"/>
-      <c r="C151" s="72"/>
+      <c r="C151" s="65"/>
       <c r="D151" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6558,13 +6498,13 @@
       <c r="N151" s="10"/>
       <c r="O151" s="10"/>
       <c r="P151" s="10"/>
-      <c r="Q151" s="66"/>
+      <c r="Q151" s="62"/>
       <c r="R151" s="60"/>
     </row>
     <row r="152" spans="1:18" ht="15.75">
       <c r="A152" s="16"/>
       <c r="B152" s="60"/>
-      <c r="C152" s="72"/>
+      <c r="C152" s="65"/>
       <c r="D152" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6593,13 +6533,13 @@
       <c r="N152" s="10"/>
       <c r="O152" s="10"/>
       <c r="P152" s="10"/>
-      <c r="Q152" s="66"/>
+      <c r="Q152" s="62"/>
       <c r="R152" s="60"/>
     </row>
     <row r="153" spans="1:18" ht="15.75">
       <c r="A153" s="16"/>
       <c r="B153" s="60"/>
-      <c r="C153" s="72"/>
+      <c r="C153" s="65"/>
       <c r="D153" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6628,13 +6568,13 @@
       <c r="N153" s="10"/>
       <c r="O153" s="10"/>
       <c r="P153" s="10"/>
-      <c r="Q153" s="67"/>
+      <c r="Q153" s="63"/>
       <c r="R153" s="60"/>
     </row>
     <row r="154" spans="1:18" ht="102" customHeight="1">
       <c r="A154" s="22"/>
-      <c r="B154" s="66"/>
-      <c r="C154" s="68"/>
+      <c r="B154" s="62"/>
+      <c r="C154" s="64"/>
       <c r="D154" s="23" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6663,13 +6603,13 @@
       <c r="N154" s="10"/>
       <c r="O154" s="10"/>
       <c r="P154" s="10"/>
-      <c r="Q154" s="65"/>
+      <c r="Q154" s="61"/>
       <c r="R154" s="60"/>
     </row>
     <row r="155" spans="1:18" ht="15.75">
       <c r="A155" s="22"/>
-      <c r="B155" s="66"/>
-      <c r="C155" s="68"/>
+      <c r="B155" s="62"/>
+      <c r="C155" s="64"/>
       <c r="D155" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6698,13 +6638,13 @@
       <c r="N155" s="10"/>
       <c r="O155" s="10"/>
       <c r="P155" s="10"/>
-      <c r="Q155" s="66"/>
+      <c r="Q155" s="62"/>
       <c r="R155" s="60"/>
     </row>
     <row r="156" spans="1:18" ht="15.75">
       <c r="A156" s="22"/>
-      <c r="B156" s="66"/>
-      <c r="C156" s="68"/>
+      <c r="B156" s="62"/>
+      <c r="C156" s="64"/>
       <c r="D156" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6733,13 +6673,13 @@
       <c r="N156" s="10"/>
       <c r="O156" s="10"/>
       <c r="P156" s="10"/>
-      <c r="Q156" s="66"/>
+      <c r="Q156" s="62"/>
       <c r="R156" s="60"/>
     </row>
     <row r="157" spans="1:18" ht="15.75">
       <c r="A157" s="22"/>
-      <c r="B157" s="66"/>
-      <c r="C157" s="68"/>
+      <c r="B157" s="62"/>
+      <c r="C157" s="64"/>
       <c r="D157" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6768,13 +6708,13 @@
       <c r="N157" s="10"/>
       <c r="O157" s="10"/>
       <c r="P157" s="10"/>
-      <c r="Q157" s="66"/>
+      <c r="Q157" s="62"/>
       <c r="R157" s="60"/>
     </row>
     <row r="158" spans="1:18" ht="15.75">
       <c r="A158" s="22"/>
-      <c r="B158" s="66"/>
-      <c r="C158" s="68"/>
+      <c r="B158" s="62"/>
+      <c r="C158" s="64"/>
       <c r="D158" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6803,13 +6743,13 @@
       <c r="N158" s="10"/>
       <c r="O158" s="10"/>
       <c r="P158" s="10"/>
-      <c r="Q158" s="66"/>
+      <c r="Q158" s="62"/>
       <c r="R158" s="60"/>
     </row>
     <row r="159" spans="1:18" ht="15.75">
       <c r="A159" s="22"/>
-      <c r="B159" s="66"/>
-      <c r="C159" s="68"/>
+      <c r="B159" s="62"/>
+      <c r="C159" s="64"/>
       <c r="D159" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6838,13 +6778,13 @@
       <c r="N159" s="10"/>
       <c r="O159" s="10"/>
       <c r="P159" s="10"/>
-      <c r="Q159" s="66"/>
+      <c r="Q159" s="62"/>
       <c r="R159" s="60"/>
     </row>
     <row r="160" spans="1:18" ht="15.75">
       <c r="A160" s="22"/>
-      <c r="B160" s="66"/>
-      <c r="C160" s="68"/>
+      <c r="B160" s="62"/>
+      <c r="C160" s="64"/>
       <c r="D160" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6873,13 +6813,13 @@
       <c r="N160" s="10"/>
       <c r="O160" s="10"/>
       <c r="P160" s="10"/>
-      <c r="Q160" s="66"/>
+      <c r="Q160" s="62"/>
       <c r="R160" s="60"/>
     </row>
     <row r="161" spans="1:18" ht="15.75">
       <c r="A161" s="22"/>
-      <c r="B161" s="66"/>
-      <c r="C161" s="68"/>
+      <c r="B161" s="62"/>
+      <c r="C161" s="64"/>
       <c r="D161" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6908,13 +6848,13 @@
       <c r="N161" s="10"/>
       <c r="O161" s="10"/>
       <c r="P161" s="10"/>
-      <c r="Q161" s="66"/>
+      <c r="Q161" s="62"/>
       <c r="R161" s="60"/>
     </row>
     <row r="162" spans="1:18" ht="15.75">
       <c r="A162" s="22"/>
-      <c r="B162" s="66"/>
-      <c r="C162" s="68"/>
+      <c r="B162" s="62"/>
+      <c r="C162" s="64"/>
       <c r="D162" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6943,13 +6883,13 @@
       <c r="N162" s="10"/>
       <c r="O162" s="10"/>
       <c r="P162" s="10"/>
-      <c r="Q162" s="66"/>
+      <c r="Q162" s="62"/>
       <c r="R162" s="60"/>
     </row>
     <row r="163" spans="1:18" ht="15.75">
       <c r="A163" s="22"/>
-      <c r="B163" s="66"/>
-      <c r="C163" s="68"/>
+      <c r="B163" s="62"/>
+      <c r="C163" s="64"/>
       <c r="D163" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -6978,13 +6918,13 @@
       <c r="N163" s="10"/>
       <c r="O163" s="10"/>
       <c r="P163" s="10"/>
-      <c r="Q163" s="66"/>
+      <c r="Q163" s="62"/>
       <c r="R163" s="60"/>
     </row>
     <row r="164" spans="1:18" ht="15.75">
       <c r="A164" s="22"/>
-      <c r="B164" s="66"/>
-      <c r="C164" s="68"/>
+      <c r="B164" s="62"/>
+      <c r="C164" s="64"/>
       <c r="D164" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7013,13 +6953,13 @@
       <c r="N164" s="10"/>
       <c r="O164" s="10"/>
       <c r="P164" s="10"/>
-      <c r="Q164" s="66"/>
+      <c r="Q164" s="62"/>
       <c r="R164" s="60"/>
     </row>
     <row r="165" spans="1:18" ht="15.75">
       <c r="A165" s="22"/>
-      <c r="B165" s="66"/>
-      <c r="C165" s="68"/>
+      <c r="B165" s="62"/>
+      <c r="C165" s="64"/>
       <c r="D165" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7048,13 +6988,13 @@
       <c r="N165" s="10"/>
       <c r="O165" s="10"/>
       <c r="P165" s="10"/>
-      <c r="Q165" s="66"/>
+      <c r="Q165" s="62"/>
       <c r="R165" s="60"/>
     </row>
     <row r="166" spans="1:18" ht="15.75">
       <c r="A166" s="22"/>
-      <c r="B166" s="66"/>
-      <c r="C166" s="68"/>
+      <c r="B166" s="62"/>
+      <c r="C166" s="64"/>
       <c r="D166" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7083,13 +7023,13 @@
       <c r="N166" s="10"/>
       <c r="O166" s="10"/>
       <c r="P166" s="10"/>
-      <c r="Q166" s="66"/>
+      <c r="Q166" s="62"/>
       <c r="R166" s="60"/>
     </row>
     <row r="167" spans="1:18" ht="15.75">
       <c r="A167" s="22"/>
-      <c r="B167" s="66"/>
-      <c r="C167" s="68"/>
+      <c r="B167" s="62"/>
+      <c r="C167" s="64"/>
       <c r="D167" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7118,13 +7058,13 @@
       <c r="N167" s="10"/>
       <c r="O167" s="10"/>
       <c r="P167" s="10"/>
-      <c r="Q167" s="66"/>
+      <c r="Q167" s="62"/>
       <c r="R167" s="60"/>
     </row>
     <row r="168" spans="1:18" ht="15.75">
       <c r="A168" s="22"/>
-      <c r="B168" s="67"/>
-      <c r="C168" s="68"/>
+      <c r="B168" s="63"/>
+      <c r="C168" s="64"/>
       <c r="D168" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7153,13 +7093,13 @@
       <c r="N168" s="10"/>
       <c r="O168" s="10"/>
       <c r="P168" s="10"/>
-      <c r="Q168" s="67"/>
+      <c r="Q168" s="63"/>
       <c r="R168" s="60"/>
     </row>
     <row r="169" spans="1:18" ht="15.75">
       <c r="A169" s="22"/>
-      <c r="B169" s="65"/>
-      <c r="C169" s="68"/>
+      <c r="B169" s="61"/>
+      <c r="C169" s="64"/>
       <c r="D169" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7188,13 +7128,13 @@
       <c r="N169" s="10"/>
       <c r="O169" s="10"/>
       <c r="P169" s="10"/>
-      <c r="Q169" s="65"/>
+      <c r="Q169" s="61"/>
       <c r="R169" s="60"/>
     </row>
     <row r="170" spans="1:18" ht="15.75">
       <c r="A170" s="22"/>
-      <c r="B170" s="66"/>
-      <c r="C170" s="68"/>
+      <c r="B170" s="62"/>
+      <c r="C170" s="64"/>
       <c r="D170" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7223,13 +7163,13 @@
       <c r="N170" s="10"/>
       <c r="O170" s="10"/>
       <c r="P170" s="10"/>
-      <c r="Q170" s="66"/>
+      <c r="Q170" s="62"/>
       <c r="R170" s="60"/>
     </row>
     <row r="171" spans="1:18" ht="15.75">
       <c r="A171" s="22"/>
-      <c r="B171" s="66"/>
-      <c r="C171" s="68"/>
+      <c r="B171" s="62"/>
+      <c r="C171" s="64"/>
       <c r="D171" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7258,13 +7198,13 @@
       <c r="N171" s="10"/>
       <c r="O171" s="10"/>
       <c r="P171" s="10"/>
-      <c r="Q171" s="66"/>
+      <c r="Q171" s="62"/>
       <c r="R171" s="60"/>
     </row>
     <row r="172" spans="1:18" ht="15.75">
       <c r="A172" s="22"/>
-      <c r="B172" s="66"/>
-      <c r="C172" s="68"/>
+      <c r="B172" s="62"/>
+      <c r="C172" s="64"/>
       <c r="D172" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7293,13 +7233,13 @@
       <c r="N172" s="10"/>
       <c r="O172" s="10"/>
       <c r="P172" s="10"/>
-      <c r="Q172" s="66"/>
+      <c r="Q172" s="62"/>
       <c r="R172" s="60"/>
     </row>
     <row r="173" spans="1:18" ht="15.75">
       <c r="A173" s="22"/>
-      <c r="B173" s="66"/>
-      <c r="C173" s="68"/>
+      <c r="B173" s="62"/>
+      <c r="C173" s="64"/>
       <c r="D173" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7328,13 +7268,13 @@
       <c r="N173" s="10"/>
       <c r="O173" s="10"/>
       <c r="P173" s="10"/>
-      <c r="Q173" s="66"/>
+      <c r="Q173" s="62"/>
       <c r="R173" s="60"/>
     </row>
     <row r="174" spans="1:18" ht="28.5" customHeight="1">
       <c r="A174" s="22"/>
-      <c r="B174" s="66"/>
-      <c r="C174" s="68"/>
+      <c r="B174" s="62"/>
+      <c r="C174" s="64"/>
       <c r="D174" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7363,13 +7303,13 @@
       <c r="N174" s="10"/>
       <c r="O174" s="10"/>
       <c r="P174" s="10"/>
-      <c r="Q174" s="66"/>
+      <c r="Q174" s="62"/>
       <c r="R174" s="60"/>
     </row>
     <row r="175" spans="1:18" ht="33.75" customHeight="1">
       <c r="A175" s="22"/>
-      <c r="B175" s="66"/>
-      <c r="C175" s="68"/>
+      <c r="B175" s="62"/>
+      <c r="C175" s="64"/>
       <c r="D175" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7398,13 +7338,13 @@
       <c r="N175" s="10"/>
       <c r="O175" s="10"/>
       <c r="P175" s="10"/>
-      <c r="Q175" s="66"/>
+      <c r="Q175" s="62"/>
       <c r="R175" s="60"/>
     </row>
     <row r="176" spans="1:18" ht="15.75">
       <c r="A176" s="22"/>
-      <c r="B176" s="66"/>
-      <c r="C176" s="68"/>
+      <c r="B176" s="62"/>
+      <c r="C176" s="64"/>
       <c r="D176" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7433,13 +7373,13 @@
       <c r="N176" s="10"/>
       <c r="O176" s="10"/>
       <c r="P176" s="10"/>
-      <c r="Q176" s="66"/>
+      <c r="Q176" s="62"/>
       <c r="R176" s="60"/>
     </row>
     <row r="177" spans="1:18" ht="15.75">
       <c r="A177" s="22"/>
-      <c r="B177" s="66"/>
-      <c r="C177" s="68"/>
+      <c r="B177" s="62"/>
+      <c r="C177" s="64"/>
       <c r="D177" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7468,13 +7408,13 @@
       <c r="N177" s="10"/>
       <c r="O177" s="10"/>
       <c r="P177" s="10"/>
-      <c r="Q177" s="66"/>
+      <c r="Q177" s="62"/>
       <c r="R177" s="60"/>
     </row>
     <row r="178" spans="1:18" ht="15.75">
       <c r="A178" s="22"/>
-      <c r="B178" s="66"/>
-      <c r="C178" s="68"/>
+      <c r="B178" s="62"/>
+      <c r="C178" s="64"/>
       <c r="D178" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7503,13 +7443,13 @@
       <c r="N178" s="10"/>
       <c r="O178" s="10"/>
       <c r="P178" s="10"/>
-      <c r="Q178" s="66"/>
+      <c r="Q178" s="62"/>
       <c r="R178" s="60"/>
     </row>
     <row r="179" spans="1:18" ht="15.75">
       <c r="A179" s="22"/>
-      <c r="B179" s="66"/>
-      <c r="C179" s="68"/>
+      <c r="B179" s="62"/>
+      <c r="C179" s="64"/>
       <c r="D179" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7538,13 +7478,13 @@
       <c r="N179" s="10"/>
       <c r="O179" s="10"/>
       <c r="P179" s="10"/>
-      <c r="Q179" s="66"/>
+      <c r="Q179" s="62"/>
       <c r="R179" s="60"/>
     </row>
     <row r="180" spans="1:18" ht="15.75">
       <c r="A180" s="22"/>
-      <c r="B180" s="66"/>
-      <c r="C180" s="68"/>
+      <c r="B180" s="62"/>
+      <c r="C180" s="64"/>
       <c r="D180" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7573,13 +7513,13 @@
       <c r="N180" s="10"/>
       <c r="O180" s="10"/>
       <c r="P180" s="10"/>
-      <c r="Q180" s="66"/>
+      <c r="Q180" s="62"/>
       <c r="R180" s="60"/>
     </row>
     <row r="181" spans="1:18" ht="15.75">
       <c r="A181" s="22"/>
-      <c r="B181" s="66"/>
-      <c r="C181" s="68"/>
+      <c r="B181" s="62"/>
+      <c r="C181" s="64"/>
       <c r="D181" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7608,13 +7548,13 @@
       <c r="N181" s="10"/>
       <c r="O181" s="10"/>
       <c r="P181" s="10"/>
-      <c r="Q181" s="66"/>
+      <c r="Q181" s="62"/>
       <c r="R181" s="60"/>
     </row>
     <row r="182" spans="1:18" ht="15.75">
       <c r="A182" s="22"/>
-      <c r="B182" s="66"/>
-      <c r="C182" s="68"/>
+      <c r="B182" s="62"/>
+      <c r="C182" s="64"/>
       <c r="D182" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7643,13 +7583,13 @@
       <c r="N182" s="10"/>
       <c r="O182" s="10"/>
       <c r="P182" s="10"/>
-      <c r="Q182" s="66"/>
+      <c r="Q182" s="62"/>
       <c r="R182" s="60"/>
     </row>
     <row r="183" spans="1:18" ht="15.75">
       <c r="A183" s="22"/>
-      <c r="B183" s="67"/>
-      <c r="C183" s="68"/>
+      <c r="B183" s="63"/>
+      <c r="C183" s="64"/>
       <c r="D183" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7678,13 +7618,13 @@
       <c r="N183" s="10"/>
       <c r="O183" s="10"/>
       <c r="P183" s="10"/>
-      <c r="Q183" s="67"/>
+      <c r="Q183" s="63"/>
       <c r="R183" s="60"/>
     </row>
     <row r="184" spans="1:18" ht="38.25" customHeight="1">
       <c r="A184" s="22"/>
-      <c r="B184" s="65"/>
-      <c r="C184" s="68"/>
+      <c r="B184" s="61"/>
+      <c r="C184" s="64"/>
       <c r="D184" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7713,13 +7653,13 @@
       <c r="N184" s="10"/>
       <c r="O184" s="10"/>
       <c r="P184" s="10"/>
-      <c r="Q184" s="65"/>
+      <c r="Q184" s="61"/>
       <c r="R184" s="60"/>
     </row>
     <row r="185" spans="1:18" ht="15.75">
       <c r="A185" s="22"/>
-      <c r="B185" s="66"/>
-      <c r="C185" s="68"/>
+      <c r="B185" s="62"/>
+      <c r="C185" s="64"/>
       <c r="D185" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7748,13 +7688,13 @@
       <c r="N185" s="10"/>
       <c r="O185" s="10"/>
       <c r="P185" s="10"/>
-      <c r="Q185" s="66"/>
+      <c r="Q185" s="62"/>
       <c r="R185" s="60"/>
     </row>
     <row r="186" spans="1:18" ht="15.75">
       <c r="A186" s="22"/>
-      <c r="B186" s="66"/>
-      <c r="C186" s="68"/>
+      <c r="B186" s="62"/>
+      <c r="C186" s="64"/>
       <c r="D186" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7783,13 +7723,13 @@
       <c r="N186" s="10"/>
       <c r="O186" s="10"/>
       <c r="P186" s="10"/>
-      <c r="Q186" s="66"/>
+      <c r="Q186" s="62"/>
       <c r="R186" s="60"/>
     </row>
     <row r="187" spans="1:18" ht="15.75">
       <c r="A187" s="22"/>
-      <c r="B187" s="66"/>
-      <c r="C187" s="68"/>
+      <c r="B187" s="62"/>
+      <c r="C187" s="64"/>
       <c r="D187" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7818,13 +7758,13 @@
       <c r="N187" s="10"/>
       <c r="O187" s="10"/>
       <c r="P187" s="10"/>
-      <c r="Q187" s="66"/>
+      <c r="Q187" s="62"/>
       <c r="R187" s="60"/>
     </row>
     <row r="188" spans="1:18" ht="15.75">
       <c r="A188" s="22"/>
-      <c r="B188" s="66"/>
-      <c r="C188" s="68"/>
+      <c r="B188" s="62"/>
+      <c r="C188" s="64"/>
       <c r="D188" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7853,13 +7793,13 @@
       <c r="N188" s="10"/>
       <c r="O188" s="10"/>
       <c r="P188" s="10"/>
-      <c r="Q188" s="66"/>
+      <c r="Q188" s="62"/>
       <c r="R188" s="60"/>
     </row>
     <row r="189" spans="1:18" ht="15.75">
       <c r="A189" s="22"/>
-      <c r="B189" s="66"/>
-      <c r="C189" s="68"/>
+      <c r="B189" s="62"/>
+      <c r="C189" s="64"/>
       <c r="D189" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7888,13 +7828,13 @@
       <c r="N189" s="10"/>
       <c r="O189" s="10"/>
       <c r="P189" s="10"/>
-      <c r="Q189" s="66"/>
+      <c r="Q189" s="62"/>
       <c r="R189" s="60"/>
     </row>
     <row r="190" spans="1:18" ht="15.75">
       <c r="A190" s="22"/>
-      <c r="B190" s="66"/>
-      <c r="C190" s="68"/>
+      <c r="B190" s="62"/>
+      <c r="C190" s="64"/>
       <c r="D190" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7923,13 +7863,13 @@
       <c r="N190" s="10"/>
       <c r="O190" s="10"/>
       <c r="P190" s="10"/>
-      <c r="Q190" s="66"/>
+      <c r="Q190" s="62"/>
       <c r="R190" s="60"/>
     </row>
     <row r="191" spans="1:18" ht="27.75" customHeight="1">
       <c r="A191" s="22"/>
-      <c r="B191" s="66"/>
-      <c r="C191" s="68"/>
+      <c r="B191" s="62"/>
+      <c r="C191" s="64"/>
       <c r="D191" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7958,13 +7898,13 @@
       <c r="N191" s="10"/>
       <c r="O191" s="10"/>
       <c r="P191" s="10"/>
-      <c r="Q191" s="66"/>
+      <c r="Q191" s="62"/>
       <c r="R191" s="60"/>
     </row>
     <row r="192" spans="1:18" ht="15.75">
       <c r="A192" s="22"/>
-      <c r="B192" s="66"/>
-      <c r="C192" s="68"/>
+      <c r="B192" s="62"/>
+      <c r="C192" s="64"/>
       <c r="D192" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -7993,13 +7933,13 @@
       <c r="N192" s="10"/>
       <c r="O192" s="10"/>
       <c r="P192" s="10"/>
-      <c r="Q192" s="66"/>
+      <c r="Q192" s="62"/>
       <c r="R192" s="60"/>
     </row>
     <row r="193" spans="1:18" ht="15.75">
       <c r="A193" s="22"/>
-      <c r="B193" s="66"/>
-      <c r="C193" s="68"/>
+      <c r="B193" s="62"/>
+      <c r="C193" s="64"/>
       <c r="D193" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -8027,13 +7967,13 @@
       <c r="N193" s="10"/>
       <c r="O193" s="10"/>
       <c r="P193" s="10"/>
-      <c r="Q193" s="66"/>
+      <c r="Q193" s="62"/>
       <c r="R193" s="60"/>
     </row>
     <row r="194" spans="1:18" ht="15.75">
       <c r="A194" s="22"/>
-      <c r="B194" s="66"/>
-      <c r="C194" s="68"/>
+      <c r="B194" s="62"/>
+      <c r="C194" s="64"/>
       <c r="D194" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -8062,13 +8002,13 @@
       <c r="N194" s="10"/>
       <c r="O194" s="10"/>
       <c r="P194" s="10"/>
-      <c r="Q194" s="66"/>
+      <c r="Q194" s="62"/>
       <c r="R194" s="60"/>
     </row>
     <row r="195" spans="1:18" ht="15.75">
       <c r="A195" s="22"/>
-      <c r="B195" s="66"/>
-      <c r="C195" s="68"/>
+      <c r="B195" s="62"/>
+      <c r="C195" s="64"/>
       <c r="D195" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -8097,13 +8037,13 @@
       <c r="N195" s="10"/>
       <c r="O195" s="10"/>
       <c r="P195" s="10"/>
-      <c r="Q195" s="66"/>
+      <c r="Q195" s="62"/>
       <c r="R195" s="60"/>
     </row>
     <row r="196" spans="1:18" ht="15.75">
       <c r="A196" s="22"/>
-      <c r="B196" s="66"/>
-      <c r="C196" s="68"/>
+      <c r="B196" s="62"/>
+      <c r="C196" s="64"/>
       <c r="D196" s="5" t="str">
         <f t="shared" si="8"/>
         <v>-</v>
@@ -8132,13 +8072,13 @@
       <c r="N196" s="10"/>
       <c r="O196" s="10"/>
       <c r="P196" s="10"/>
-      <c r="Q196" s="66"/>
+      <c r="Q196" s="62"/>
       <c r="R196" s="60"/>
     </row>
     <row r="197" spans="1:18" ht="15.75">
       <c r="A197" s="22"/>
-      <c r="B197" s="66"/>
-      <c r="C197" s="68"/>
+      <c r="B197" s="62"/>
+      <c r="C197" s="64"/>
       <c r="D197" s="5" t="str">
         <f t="shared" ref="D197:D260" si="12">IF(LEN(E197)&gt;5,IF(LEN(K197&amp;L197&amp;M197)&gt;=1,"OK","Check"),"-")</f>
         <v>-</v>
@@ -8167,13 +8107,13 @@
       <c r="N197" s="10"/>
       <c r="O197" s="10"/>
       <c r="P197" s="10"/>
-      <c r="Q197" s="66"/>
+      <c r="Q197" s="62"/>
       <c r="R197" s="60"/>
     </row>
     <row r="198" spans="1:18" ht="15.75">
       <c r="A198" s="22"/>
-      <c r="B198" s="67"/>
-      <c r="C198" s="68"/>
+      <c r="B198" s="63"/>
+      <c r="C198" s="64"/>
       <c r="D198" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8202,13 +8142,13 @@
       <c r="N198" s="10"/>
       <c r="O198" s="10"/>
       <c r="P198" s="10"/>
-      <c r="Q198" s="67"/>
+      <c r="Q198" s="63"/>
       <c r="R198" s="60"/>
     </row>
     <row r="199" spans="1:18" ht="25.5" customHeight="1">
       <c r="A199" s="22"/>
-      <c r="B199" s="65"/>
-      <c r="C199" s="68"/>
+      <c r="B199" s="61"/>
+      <c r="C199" s="64"/>
       <c r="D199" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8237,13 +8177,13 @@
       <c r="N199" s="10"/>
       <c r="O199" s="10"/>
       <c r="P199" s="10"/>
-      <c r="Q199" s="65"/>
+      <c r="Q199" s="61"/>
       <c r="R199" s="60"/>
     </row>
     <row r="200" spans="1:18" ht="15.75">
       <c r="A200" s="22"/>
-      <c r="B200" s="66"/>
-      <c r="C200" s="68"/>
+      <c r="B200" s="62"/>
+      <c r="C200" s="64"/>
       <c r="D200" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8272,13 +8212,13 @@
       <c r="N200" s="10"/>
       <c r="O200" s="10"/>
       <c r="P200" s="10"/>
-      <c r="Q200" s="66"/>
+      <c r="Q200" s="62"/>
       <c r="R200" s="60"/>
     </row>
     <row r="201" spans="1:18" ht="15.75">
       <c r="A201" s="22"/>
-      <c r="B201" s="66"/>
-      <c r="C201" s="68"/>
+      <c r="B201" s="62"/>
+      <c r="C201" s="64"/>
       <c r="D201" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8307,13 +8247,13 @@
       <c r="N201" s="10"/>
       <c r="O201" s="10"/>
       <c r="P201" s="10"/>
-      <c r="Q201" s="66"/>
+      <c r="Q201" s="62"/>
       <c r="R201" s="60"/>
     </row>
     <row r="202" spans="1:18" ht="15.75">
       <c r="A202" s="22"/>
-      <c r="B202" s="66"/>
-      <c r="C202" s="68"/>
+      <c r="B202" s="62"/>
+      <c r="C202" s="64"/>
       <c r="D202" s="33" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8342,13 +8282,13 @@
       <c r="N202" s="10"/>
       <c r="O202" s="10"/>
       <c r="P202" s="10"/>
-      <c r="Q202" s="66"/>
+      <c r="Q202" s="62"/>
       <c r="R202" s="60"/>
     </row>
     <row r="203" spans="1:18" ht="15.75">
       <c r="A203" s="22"/>
-      <c r="B203" s="66"/>
-      <c r="C203" s="68"/>
+      <c r="B203" s="62"/>
+      <c r="C203" s="64"/>
       <c r="D203" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8377,13 +8317,13 @@
       <c r="N203" s="10"/>
       <c r="O203" s="10"/>
       <c r="P203" s="10"/>
-      <c r="Q203" s="66"/>
+      <c r="Q203" s="62"/>
       <c r="R203" s="60"/>
     </row>
     <row r="204" spans="1:18" ht="15.75">
       <c r="A204" s="22"/>
-      <c r="B204" s="66"/>
-      <c r="C204" s="68"/>
+      <c r="B204" s="62"/>
+      <c r="C204" s="64"/>
       <c r="D204" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8412,13 +8352,13 @@
       <c r="N204" s="10"/>
       <c r="O204" s="10"/>
       <c r="P204" s="10"/>
-      <c r="Q204" s="66"/>
+      <c r="Q204" s="62"/>
       <c r="R204" s="60"/>
     </row>
     <row r="205" spans="1:18" ht="15.75">
       <c r="A205" s="22"/>
-      <c r="B205" s="66"/>
-      <c r="C205" s="68"/>
+      <c r="B205" s="62"/>
+      <c r="C205" s="64"/>
       <c r="D205" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8447,13 +8387,13 @@
       <c r="N205" s="10"/>
       <c r="O205" s="10"/>
       <c r="P205" s="10"/>
-      <c r="Q205" s="66"/>
+      <c r="Q205" s="62"/>
       <c r="R205" s="60"/>
     </row>
     <row r="206" spans="1:18" ht="15.75">
       <c r="A206" s="22"/>
-      <c r="B206" s="66"/>
-      <c r="C206" s="68"/>
+      <c r="B206" s="62"/>
+      <c r="C206" s="64"/>
       <c r="D206" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8482,13 +8422,13 @@
       <c r="N206" s="10"/>
       <c r="O206" s="10"/>
       <c r="P206" s="10"/>
-      <c r="Q206" s="66"/>
+      <c r="Q206" s="62"/>
       <c r="R206" s="60"/>
     </row>
     <row r="207" spans="1:18" ht="15.75">
       <c r="A207" s="22"/>
-      <c r="B207" s="66"/>
-      <c r="C207" s="68"/>
+      <c r="B207" s="62"/>
+      <c r="C207" s="64"/>
       <c r="D207" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8517,13 +8457,13 @@
       <c r="N207" s="10"/>
       <c r="O207" s="10"/>
       <c r="P207" s="10"/>
-      <c r="Q207" s="66"/>
+      <c r="Q207" s="62"/>
       <c r="R207" s="60"/>
     </row>
     <row r="208" spans="1:18" ht="15.75">
       <c r="A208" s="22"/>
-      <c r="B208" s="66"/>
-      <c r="C208" s="68"/>
+      <c r="B208" s="62"/>
+      <c r="C208" s="64"/>
       <c r="D208" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8552,13 +8492,13 @@
       <c r="N208" s="10"/>
       <c r="O208" s="10"/>
       <c r="P208" s="10"/>
-      <c r="Q208" s="66"/>
+      <c r="Q208" s="62"/>
       <c r="R208" s="60"/>
     </row>
     <row r="209" spans="1:18" ht="15.75">
       <c r="A209" s="22"/>
-      <c r="B209" s="66"/>
-      <c r="C209" s="68"/>
+      <c r="B209" s="62"/>
+      <c r="C209" s="64"/>
       <c r="D209" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8587,13 +8527,13 @@
       <c r="N209" s="10"/>
       <c r="O209" s="10"/>
       <c r="P209" s="10"/>
-      <c r="Q209" s="66"/>
+      <c r="Q209" s="62"/>
       <c r="R209" s="60"/>
     </row>
     <row r="210" spans="1:18" ht="15.75">
       <c r="A210" s="22"/>
-      <c r="B210" s="66"/>
-      <c r="C210" s="68"/>
+      <c r="B210" s="62"/>
+      <c r="C210" s="64"/>
       <c r="D210" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8622,13 +8562,13 @@
       <c r="N210" s="10"/>
       <c r="O210" s="10"/>
       <c r="P210" s="10"/>
-      <c r="Q210" s="66"/>
+      <c r="Q210" s="62"/>
       <c r="R210" s="60"/>
     </row>
     <row r="211" spans="1:18" ht="15.75">
       <c r="A211" s="22"/>
-      <c r="B211" s="66"/>
-      <c r="C211" s="68"/>
+      <c r="B211" s="62"/>
+      <c r="C211" s="64"/>
       <c r="D211" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8657,13 +8597,13 @@
       <c r="N211" s="10"/>
       <c r="O211" s="10"/>
       <c r="P211" s="10"/>
-      <c r="Q211" s="66"/>
+      <c r="Q211" s="62"/>
       <c r="R211" s="60"/>
     </row>
     <row r="212" spans="1:18" ht="15.75">
       <c r="A212" s="22"/>
-      <c r="B212" s="66"/>
-      <c r="C212" s="68"/>
+      <c r="B212" s="62"/>
+      <c r="C212" s="64"/>
       <c r="D212" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8692,13 +8632,13 @@
       <c r="N212" s="10"/>
       <c r="O212" s="10"/>
       <c r="P212" s="10"/>
-      <c r="Q212" s="66"/>
+      <c r="Q212" s="62"/>
       <c r="R212" s="60"/>
     </row>
     <row r="213" spans="1:18" ht="15.75">
       <c r="A213" s="22"/>
-      <c r="B213" s="67"/>
-      <c r="C213" s="68"/>
+      <c r="B213" s="63"/>
+      <c r="C213" s="64"/>
       <c r="D213" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8727,13 +8667,13 @@
       <c r="N213" s="10"/>
       <c r="O213" s="10"/>
       <c r="P213" s="10"/>
-      <c r="Q213" s="67"/>
+      <c r="Q213" s="63"/>
       <c r="R213" s="60"/>
     </row>
     <row r="214" spans="1:18" ht="12.75" customHeight="1">
       <c r="A214" s="22"/>
-      <c r="B214" s="65"/>
-      <c r="C214" s="68"/>
+      <c r="B214" s="61"/>
+      <c r="C214" s="64"/>
       <c r="D214" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8762,13 +8702,13 @@
       <c r="N214" s="10"/>
       <c r="O214" s="10"/>
       <c r="P214" s="10"/>
-      <c r="Q214" s="65"/>
+      <c r="Q214" s="61"/>
       <c r="R214" s="60"/>
     </row>
     <row r="215" spans="1:18" ht="15.75">
       <c r="A215" s="22"/>
-      <c r="B215" s="66"/>
-      <c r="C215" s="68"/>
+      <c r="B215" s="62"/>
+      <c r="C215" s="64"/>
       <c r="D215" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8797,13 +8737,13 @@
       <c r="N215" s="10"/>
       <c r="O215" s="10"/>
       <c r="P215" s="10"/>
-      <c r="Q215" s="66"/>
+      <c r="Q215" s="62"/>
       <c r="R215" s="60"/>
     </row>
     <row r="216" spans="1:18" ht="15.75">
       <c r="A216" s="22"/>
-      <c r="B216" s="66"/>
-      <c r="C216" s="68"/>
+      <c r="B216" s="62"/>
+      <c r="C216" s="64"/>
       <c r="D216" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8832,13 +8772,13 @@
       <c r="N216" s="10"/>
       <c r="O216" s="10"/>
       <c r="P216" s="10"/>
-      <c r="Q216" s="66"/>
+      <c r="Q216" s="62"/>
       <c r="R216" s="60"/>
     </row>
     <row r="217" spans="1:18" ht="15.75">
       <c r="A217" s="22"/>
-      <c r="B217" s="66"/>
-      <c r="C217" s="68"/>
+      <c r="B217" s="62"/>
+      <c r="C217" s="64"/>
       <c r="D217" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8867,13 +8807,13 @@
       <c r="N217" s="10"/>
       <c r="O217" s="10"/>
       <c r="P217" s="10"/>
-      <c r="Q217" s="66"/>
+      <c r="Q217" s="62"/>
       <c r="R217" s="60"/>
     </row>
     <row r="218" spans="1:18" ht="15.75">
       <c r="A218" s="22"/>
-      <c r="B218" s="66"/>
-      <c r="C218" s="68"/>
+      <c r="B218" s="62"/>
+      <c r="C218" s="64"/>
       <c r="D218" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8902,13 +8842,13 @@
       <c r="N218" s="10"/>
       <c r="O218" s="10"/>
       <c r="P218" s="10"/>
-      <c r="Q218" s="66"/>
+      <c r="Q218" s="62"/>
       <c r="R218" s="60"/>
     </row>
     <row r="219" spans="1:18" ht="15.75">
       <c r="A219" s="22"/>
-      <c r="B219" s="66"/>
-      <c r="C219" s="68"/>
+      <c r="B219" s="62"/>
+      <c r="C219" s="64"/>
       <c r="D219" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8937,13 +8877,13 @@
       <c r="N219" s="10"/>
       <c r="O219" s="10"/>
       <c r="P219" s="10"/>
-      <c r="Q219" s="66"/>
+      <c r="Q219" s="62"/>
       <c r="R219" s="60"/>
     </row>
     <row r="220" spans="1:18" ht="15.75">
       <c r="A220" s="22"/>
-      <c r="B220" s="66"/>
-      <c r="C220" s="68"/>
+      <c r="B220" s="62"/>
+      <c r="C220" s="64"/>
       <c r="D220" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -8972,13 +8912,13 @@
       <c r="N220" s="10"/>
       <c r="O220" s="10"/>
       <c r="P220" s="10"/>
-      <c r="Q220" s="66"/>
+      <c r="Q220" s="62"/>
       <c r="R220" s="60"/>
     </row>
     <row r="221" spans="1:18" ht="15.75">
       <c r="A221" s="22"/>
-      <c r="B221" s="66"/>
-      <c r="C221" s="68"/>
+      <c r="B221" s="62"/>
+      <c r="C221" s="64"/>
       <c r="D221" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9007,13 +8947,13 @@
       <c r="N221" s="10"/>
       <c r="O221" s="10"/>
       <c r="P221" s="10"/>
-      <c r="Q221" s="66"/>
+      <c r="Q221" s="62"/>
       <c r="R221" s="60"/>
     </row>
     <row r="222" spans="1:18" ht="15.75">
       <c r="A222" s="22"/>
-      <c r="B222" s="66"/>
-      <c r="C222" s="68"/>
+      <c r="B222" s="62"/>
+      <c r="C222" s="64"/>
       <c r="D222" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9042,13 +8982,13 @@
       <c r="N222" s="10"/>
       <c r="O222" s="10"/>
       <c r="P222" s="10"/>
-      <c r="Q222" s="66"/>
+      <c r="Q222" s="62"/>
       <c r="R222" s="60"/>
     </row>
     <row r="223" spans="1:18" ht="15.75">
       <c r="A223" s="22"/>
-      <c r="B223" s="66"/>
-      <c r="C223" s="68"/>
+      <c r="B223" s="62"/>
+      <c r="C223" s="64"/>
       <c r="D223" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9077,13 +9017,13 @@
       <c r="N223" s="10"/>
       <c r="O223" s="10"/>
       <c r="P223" s="10"/>
-      <c r="Q223" s="66"/>
+      <c r="Q223" s="62"/>
       <c r="R223" s="60"/>
     </row>
     <row r="224" spans="1:18" ht="15.75">
       <c r="A224" s="22"/>
-      <c r="B224" s="66"/>
-      <c r="C224" s="68"/>
+      <c r="B224" s="62"/>
+      <c r="C224" s="64"/>
       <c r="D224" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9112,13 +9052,13 @@
       <c r="N224" s="10"/>
       <c r="O224" s="10"/>
       <c r="P224" s="10"/>
-      <c r="Q224" s="66"/>
+      <c r="Q224" s="62"/>
       <c r="R224" s="60"/>
     </row>
     <row r="225" spans="1:18" ht="15.75">
       <c r="A225" s="22"/>
-      <c r="B225" s="66"/>
-      <c r="C225" s="68"/>
+      <c r="B225" s="62"/>
+      <c r="C225" s="64"/>
       <c r="D225" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9147,13 +9087,13 @@
       <c r="N225" s="10"/>
       <c r="O225" s="10"/>
       <c r="P225" s="10"/>
-      <c r="Q225" s="66"/>
+      <c r="Q225" s="62"/>
       <c r="R225" s="60"/>
     </row>
     <row r="226" spans="1:18" ht="15.75">
       <c r="A226" s="22"/>
-      <c r="B226" s="66"/>
-      <c r="C226" s="68"/>
+      <c r="B226" s="62"/>
+      <c r="C226" s="64"/>
       <c r="D226" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9182,13 +9122,13 @@
       <c r="N226" s="10"/>
       <c r="O226" s="10"/>
       <c r="P226" s="10"/>
-      <c r="Q226" s="66"/>
+      <c r="Q226" s="62"/>
       <c r="R226" s="60"/>
     </row>
     <row r="227" spans="1:18" ht="15.75">
       <c r="A227" s="22"/>
-      <c r="B227" s="66"/>
-      <c r="C227" s="68"/>
+      <c r="B227" s="62"/>
+      <c r="C227" s="64"/>
       <c r="D227" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9217,13 +9157,13 @@
       <c r="N227" s="10"/>
       <c r="O227" s="10"/>
       <c r="P227" s="10"/>
-      <c r="Q227" s="66"/>
+      <c r="Q227" s="62"/>
       <c r="R227" s="60"/>
     </row>
     <row r="228" spans="1:18" ht="15.75">
       <c r="A228" s="22"/>
-      <c r="B228" s="67"/>
-      <c r="C228" s="68"/>
+      <c r="B228" s="63"/>
+      <c r="C228" s="64"/>
       <c r="D228" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9252,13 +9192,13 @@
       <c r="N228" s="10"/>
       <c r="O228" s="10"/>
       <c r="P228" s="10"/>
-      <c r="Q228" s="67"/>
+      <c r="Q228" s="63"/>
       <c r="R228" s="60"/>
     </row>
     <row r="229" spans="1:18" ht="25.5" customHeight="1">
       <c r="A229" s="22"/>
-      <c r="B229" s="65"/>
-      <c r="C229" s="68"/>
+      <c r="B229" s="61"/>
+      <c r="C229" s="64"/>
       <c r="D229" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9287,13 +9227,13 @@
       <c r="N229" s="10"/>
       <c r="O229" s="10"/>
       <c r="P229" s="46"/>
-      <c r="Q229" s="65"/>
+      <c r="Q229" s="61"/>
       <c r="R229" s="60"/>
     </row>
     <row r="230" spans="1:18" ht="15.75">
       <c r="A230" s="22"/>
-      <c r="B230" s="66"/>
-      <c r="C230" s="68"/>
+      <c r="B230" s="62"/>
+      <c r="C230" s="64"/>
       <c r="D230" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9322,13 +9262,13 @@
       <c r="N230" s="10"/>
       <c r="O230" s="10"/>
       <c r="P230" s="46"/>
-      <c r="Q230" s="66"/>
+      <c r="Q230" s="62"/>
       <c r="R230" s="60"/>
     </row>
     <row r="231" spans="1:18" ht="15.75">
       <c r="A231" s="22"/>
-      <c r="B231" s="66"/>
-      <c r="C231" s="68"/>
+      <c r="B231" s="62"/>
+      <c r="C231" s="64"/>
       <c r="D231" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9357,13 +9297,13 @@
       <c r="N231" s="10"/>
       <c r="O231" s="10"/>
       <c r="P231" s="10"/>
-      <c r="Q231" s="66"/>
+      <c r="Q231" s="62"/>
       <c r="R231" s="60"/>
     </row>
     <row r="232" spans="1:18" ht="15.75">
       <c r="A232" s="22"/>
-      <c r="B232" s="66"/>
-      <c r="C232" s="68"/>
+      <c r="B232" s="62"/>
+      <c r="C232" s="64"/>
       <c r="D232" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9392,13 +9332,13 @@
       <c r="N232" s="10"/>
       <c r="O232" s="10"/>
       <c r="P232" s="10"/>
-      <c r="Q232" s="66"/>
+      <c r="Q232" s="62"/>
       <c r="R232" s="60"/>
     </row>
     <row r="233" spans="1:18" ht="15.75">
       <c r="A233" s="22"/>
-      <c r="B233" s="66"/>
-      <c r="C233" s="68"/>
+      <c r="B233" s="62"/>
+      <c r="C233" s="64"/>
       <c r="D233" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9427,13 +9367,13 @@
       <c r="N233" s="10"/>
       <c r="O233" s="10"/>
       <c r="P233" s="10"/>
-      <c r="Q233" s="66"/>
+      <c r="Q233" s="62"/>
       <c r="R233" s="60"/>
     </row>
     <row r="234" spans="1:18" ht="15.75">
       <c r="A234" s="22"/>
-      <c r="B234" s="66"/>
-      <c r="C234" s="68"/>
+      <c r="B234" s="62"/>
+      <c r="C234" s="64"/>
       <c r="D234" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9462,13 +9402,13 @@
       <c r="N234" s="10"/>
       <c r="O234" s="10"/>
       <c r="P234" s="10"/>
-      <c r="Q234" s="66"/>
+      <c r="Q234" s="62"/>
       <c r="R234" s="60"/>
     </row>
     <row r="235" spans="1:18" ht="15.75">
       <c r="A235" s="22"/>
-      <c r="B235" s="66"/>
-      <c r="C235" s="68"/>
+      <c r="B235" s="62"/>
+      <c r="C235" s="64"/>
       <c r="D235" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9497,13 +9437,13 @@
       <c r="N235" s="10"/>
       <c r="O235" s="10"/>
       <c r="P235" s="10"/>
-      <c r="Q235" s="66"/>
+      <c r="Q235" s="62"/>
       <c r="R235" s="60"/>
     </row>
     <row r="236" spans="1:18" ht="15.75">
       <c r="A236" s="22"/>
-      <c r="B236" s="66"/>
-      <c r="C236" s="68"/>
+      <c r="B236" s="62"/>
+      <c r="C236" s="64"/>
       <c r="D236" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9532,13 +9472,13 @@
       <c r="N236" s="10"/>
       <c r="O236" s="10"/>
       <c r="P236" s="10"/>
-      <c r="Q236" s="66"/>
+      <c r="Q236" s="62"/>
       <c r="R236" s="60"/>
     </row>
     <row r="237" spans="1:18" ht="15.75">
       <c r="A237" s="22"/>
-      <c r="B237" s="66"/>
-      <c r="C237" s="68"/>
+      <c r="B237" s="62"/>
+      <c r="C237" s="64"/>
       <c r="D237" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9567,13 +9507,13 @@
       <c r="N237" s="10"/>
       <c r="O237" s="10"/>
       <c r="P237" s="10"/>
-      <c r="Q237" s="66"/>
+      <c r="Q237" s="62"/>
       <c r="R237" s="60"/>
     </row>
     <row r="238" spans="1:18" ht="15.75">
       <c r="A238" s="22"/>
-      <c r="B238" s="66"/>
-      <c r="C238" s="68"/>
+      <c r="B238" s="62"/>
+      <c r="C238" s="64"/>
       <c r="D238" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9602,13 +9542,13 @@
       <c r="N238" s="10"/>
       <c r="O238" s="10"/>
       <c r="P238" s="10"/>
-      <c r="Q238" s="66"/>
+      <c r="Q238" s="62"/>
       <c r="R238" s="60"/>
     </row>
     <row r="239" spans="1:18" ht="15.75">
       <c r="A239" s="22"/>
-      <c r="B239" s="66"/>
-      <c r="C239" s="68"/>
+      <c r="B239" s="62"/>
+      <c r="C239" s="64"/>
       <c r="D239" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9637,13 +9577,13 @@
       <c r="N239" s="10"/>
       <c r="O239" s="10"/>
       <c r="P239" s="10"/>
-      <c r="Q239" s="66"/>
+      <c r="Q239" s="62"/>
       <c r="R239" s="60"/>
     </row>
     <row r="240" spans="1:18" ht="15.75">
       <c r="A240" s="22"/>
-      <c r="B240" s="66"/>
-      <c r="C240" s="68"/>
+      <c r="B240" s="62"/>
+      <c r="C240" s="64"/>
       <c r="D240" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9672,13 +9612,13 @@
       <c r="N240" s="10"/>
       <c r="O240" s="10"/>
       <c r="P240" s="10"/>
-      <c r="Q240" s="66"/>
+      <c r="Q240" s="62"/>
       <c r="R240" s="60"/>
     </row>
     <row r="241" spans="1:18" ht="15.75">
       <c r="A241" s="22"/>
-      <c r="B241" s="66"/>
-      <c r="C241" s="68"/>
+      <c r="B241" s="62"/>
+      <c r="C241" s="64"/>
       <c r="D241" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9707,13 +9647,13 @@
       <c r="N241" s="10"/>
       <c r="O241" s="10"/>
       <c r="P241" s="10"/>
-      <c r="Q241" s="66"/>
+      <c r="Q241" s="62"/>
       <c r="R241" s="60"/>
     </row>
     <row r="242" spans="1:18" ht="15.75">
       <c r="A242" s="22"/>
-      <c r="B242" s="66"/>
-      <c r="C242" s="68"/>
+      <c r="B242" s="62"/>
+      <c r="C242" s="64"/>
       <c r="D242" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9742,13 +9682,13 @@
       <c r="N242" s="10"/>
       <c r="O242" s="10"/>
       <c r="P242" s="10"/>
-      <c r="Q242" s="66"/>
+      <c r="Q242" s="62"/>
       <c r="R242" s="60"/>
     </row>
     <row r="243" spans="1:18" ht="15.75">
       <c r="A243" s="22"/>
-      <c r="B243" s="67"/>
-      <c r="C243" s="68"/>
+      <c r="B243" s="63"/>
+      <c r="C243" s="64"/>
       <c r="D243" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9777,13 +9717,13 @@
       <c r="N243" s="10"/>
       <c r="O243" s="10"/>
       <c r="P243" s="10"/>
-      <c r="Q243" s="67"/>
+      <c r="Q243" s="63"/>
       <c r="R243" s="60"/>
     </row>
     <row r="244" spans="1:18" ht="15.75">
       <c r="A244" s="22"/>
-      <c r="B244" s="65"/>
-      <c r="C244" s="68"/>
+      <c r="B244" s="61"/>
+      <c r="C244" s="64"/>
       <c r="D244" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9812,13 +9752,13 @@
       <c r="N244" s="10"/>
       <c r="O244" s="10"/>
       <c r="P244" s="10"/>
-      <c r="Q244" s="65"/>
+      <c r="Q244" s="61"/>
       <c r="R244" s="60"/>
     </row>
     <row r="245" spans="1:18" ht="15.75">
       <c r="A245" s="22"/>
-      <c r="B245" s="66"/>
-      <c r="C245" s="68"/>
+      <c r="B245" s="62"/>
+      <c r="C245" s="64"/>
       <c r="D245" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9847,13 +9787,13 @@
       <c r="N245" s="10"/>
       <c r="O245" s="10"/>
       <c r="P245" s="10"/>
-      <c r="Q245" s="66"/>
+      <c r="Q245" s="62"/>
       <c r="R245" s="60"/>
     </row>
     <row r="246" spans="1:18" ht="15.75">
       <c r="A246" s="22"/>
-      <c r="B246" s="66"/>
-      <c r="C246" s="68"/>
+      <c r="B246" s="62"/>
+      <c r="C246" s="64"/>
       <c r="D246" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9882,13 +9822,13 @@
       <c r="N246" s="10"/>
       <c r="O246" s="10"/>
       <c r="P246" s="10"/>
-      <c r="Q246" s="66"/>
+      <c r="Q246" s="62"/>
       <c r="R246" s="60"/>
     </row>
     <row r="247" spans="1:18" ht="15.75">
       <c r="A247" s="22"/>
-      <c r="B247" s="66"/>
-      <c r="C247" s="68"/>
+      <c r="B247" s="62"/>
+      <c r="C247" s="64"/>
       <c r="D247" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9917,13 +9857,13 @@
       <c r="N247" s="10"/>
       <c r="O247" s="10"/>
       <c r="P247" s="10"/>
-      <c r="Q247" s="66"/>
+      <c r="Q247" s="62"/>
       <c r="R247" s="60"/>
     </row>
     <row r="248" spans="1:18" ht="15.75">
       <c r="A248" s="22"/>
-      <c r="B248" s="66"/>
-      <c r="C248" s="68"/>
+      <c r="B248" s="62"/>
+      <c r="C248" s="64"/>
       <c r="D248" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9952,13 +9892,13 @@
       <c r="N248" s="10"/>
       <c r="O248" s="10"/>
       <c r="P248" s="10"/>
-      <c r="Q248" s="66"/>
+      <c r="Q248" s="62"/>
       <c r="R248" s="60"/>
     </row>
     <row r="249" spans="1:18" ht="15.75">
       <c r="A249" s="22"/>
-      <c r="B249" s="66"/>
-      <c r="C249" s="68"/>
+      <c r="B249" s="62"/>
+      <c r="C249" s="64"/>
       <c r="D249" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -9987,13 +9927,13 @@
       <c r="N249" s="10"/>
       <c r="O249" s="10"/>
       <c r="P249" s="10"/>
-      <c r="Q249" s="66"/>
+      <c r="Q249" s="62"/>
       <c r="R249" s="60"/>
     </row>
     <row r="250" spans="1:18" ht="15.75">
       <c r="A250" s="22"/>
-      <c r="B250" s="66"/>
-      <c r="C250" s="68"/>
+      <c r="B250" s="62"/>
+      <c r="C250" s="64"/>
       <c r="D250" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10022,13 +9962,13 @@
       <c r="N250" s="10"/>
       <c r="O250" s="10"/>
       <c r="P250" s="10"/>
-      <c r="Q250" s="66"/>
+      <c r="Q250" s="62"/>
       <c r="R250" s="60"/>
     </row>
     <row r="251" spans="1:18" ht="15.75">
       <c r="A251" s="22"/>
-      <c r="B251" s="66"/>
-      <c r="C251" s="68"/>
+      <c r="B251" s="62"/>
+      <c r="C251" s="64"/>
       <c r="D251" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10057,13 +9997,13 @@
       <c r="N251" s="10"/>
       <c r="O251" s="10"/>
       <c r="P251" s="10"/>
-      <c r="Q251" s="66"/>
+      <c r="Q251" s="62"/>
       <c r="R251" s="60"/>
     </row>
     <row r="252" spans="1:18" ht="15.75">
       <c r="A252" s="22"/>
-      <c r="B252" s="66"/>
-      <c r="C252" s="68"/>
+      <c r="B252" s="62"/>
+      <c r="C252" s="64"/>
       <c r="D252" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10092,13 +10032,13 @@
       <c r="N252" s="10"/>
       <c r="O252" s="10"/>
       <c r="P252" s="10"/>
-      <c r="Q252" s="66"/>
+      <c r="Q252" s="62"/>
       <c r="R252" s="60"/>
     </row>
     <row r="253" spans="1:18" ht="15.75">
       <c r="A253" s="22"/>
-      <c r="B253" s="66"/>
-      <c r="C253" s="68"/>
+      <c r="B253" s="62"/>
+      <c r="C253" s="64"/>
       <c r="D253" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10127,13 +10067,13 @@
       <c r="N253" s="10"/>
       <c r="O253" s="10"/>
       <c r="P253" s="10"/>
-      <c r="Q253" s="66"/>
+      <c r="Q253" s="62"/>
       <c r="R253" s="60"/>
     </row>
     <row r="254" spans="1:18" ht="15.75">
       <c r="A254" s="22"/>
-      <c r="B254" s="66"/>
-      <c r="C254" s="68"/>
+      <c r="B254" s="62"/>
+      <c r="C254" s="64"/>
       <c r="D254" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10162,13 +10102,13 @@
       <c r="N254" s="10"/>
       <c r="O254" s="10"/>
       <c r="P254" s="10"/>
-      <c r="Q254" s="66"/>
+      <c r="Q254" s="62"/>
       <c r="R254" s="60"/>
     </row>
     <row r="255" spans="1:18" ht="15.75">
       <c r="A255" s="22"/>
-      <c r="B255" s="66"/>
-      <c r="C255" s="68"/>
+      <c r="B255" s="62"/>
+      <c r="C255" s="64"/>
       <c r="D255" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10197,13 +10137,13 @@
       <c r="N255" s="10"/>
       <c r="O255" s="10"/>
       <c r="P255" s="10"/>
-      <c r="Q255" s="66"/>
+      <c r="Q255" s="62"/>
       <c r="R255" s="60"/>
     </row>
     <row r="256" spans="1:18" ht="15.75">
       <c r="A256" s="22"/>
-      <c r="B256" s="66"/>
-      <c r="C256" s="68"/>
+      <c r="B256" s="62"/>
+      <c r="C256" s="64"/>
       <c r="D256" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10232,13 +10172,13 @@
       <c r="N256" s="10"/>
       <c r="O256" s="10"/>
       <c r="P256" s="10"/>
-      <c r="Q256" s="66"/>
+      <c r="Q256" s="62"/>
       <c r="R256" s="60"/>
     </row>
     <row r="257" spans="1:18" ht="15.75">
       <c r="A257" s="22"/>
-      <c r="B257" s="66"/>
-      <c r="C257" s="68"/>
+      <c r="B257" s="62"/>
+      <c r="C257" s="64"/>
       <c r="D257" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10267,13 +10207,13 @@
       <c r="N257" s="10"/>
       <c r="O257" s="10"/>
       <c r="P257" s="10"/>
-      <c r="Q257" s="66"/>
+      <c r="Q257" s="62"/>
       <c r="R257" s="60"/>
     </row>
     <row r="258" spans="1:18" ht="15.75">
       <c r="A258" s="22"/>
-      <c r="B258" s="67"/>
-      <c r="C258" s="68"/>
+      <c r="B258" s="63"/>
+      <c r="C258" s="64"/>
       <c r="D258" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10302,13 +10242,13 @@
       <c r="N258" s="47"/>
       <c r="O258" s="47"/>
       <c r="P258" s="47"/>
-      <c r="Q258" s="67"/>
+      <c r="Q258" s="63"/>
       <c r="R258" s="60"/>
     </row>
     <row r="259" spans="1:18" ht="12.75" customHeight="1">
       <c r="A259" s="22"/>
-      <c r="B259" s="65"/>
-      <c r="C259" s="68"/>
+      <c r="B259" s="61"/>
+      <c r="C259" s="64"/>
       <c r="D259" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10337,13 +10277,13 @@
       <c r="N259" s="47"/>
       <c r="O259" s="47"/>
       <c r="P259" s="47"/>
-      <c r="Q259" s="65"/>
+      <c r="Q259" s="61"/>
       <c r="R259" s="60"/>
     </row>
     <row r="260" spans="1:18" ht="15.75">
       <c r="A260" s="22"/>
-      <c r="B260" s="66"/>
-      <c r="C260" s="68"/>
+      <c r="B260" s="62"/>
+      <c r="C260" s="64"/>
       <c r="D260" s="5" t="str">
         <f t="shared" si="12"/>
         <v>-</v>
@@ -10372,13 +10312,13 @@
       <c r="N260" s="47"/>
       <c r="O260" s="47"/>
       <c r="P260" s="47"/>
-      <c r="Q260" s="66"/>
+      <c r="Q260" s="62"/>
       <c r="R260" s="60"/>
     </row>
     <row r="261" spans="1:18" ht="15.75">
       <c r="A261" s="22"/>
-      <c r="B261" s="66"/>
-      <c r="C261" s="68"/>
+      <c r="B261" s="62"/>
+      <c r="C261" s="64"/>
       <c r="D261" s="5" t="str">
         <f t="shared" ref="D261:D273" si="16">IF(LEN(E261)&gt;5,IF(LEN(K261&amp;L261&amp;M261)&gt;=1,"OK","Check"),"-")</f>
         <v>-</v>
@@ -10407,13 +10347,13 @@
       <c r="N261" s="47"/>
       <c r="O261" s="47"/>
       <c r="P261" s="47"/>
-      <c r="Q261" s="66"/>
+      <c r="Q261" s="62"/>
       <c r="R261" s="60"/>
     </row>
     <row r="262" spans="1:18" ht="15.75">
       <c r="A262" s="22"/>
-      <c r="B262" s="66"/>
-      <c r="C262" s="68"/>
+      <c r="B262" s="62"/>
+      <c r="C262" s="64"/>
       <c r="D262" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10442,13 +10382,13 @@
       <c r="N262" s="47"/>
       <c r="O262" s="47"/>
       <c r="P262" s="47"/>
-      <c r="Q262" s="66"/>
+      <c r="Q262" s="62"/>
       <c r="R262" s="60"/>
     </row>
     <row r="263" spans="1:18" ht="15.75">
       <c r="A263" s="22"/>
-      <c r="B263" s="66"/>
-      <c r="C263" s="68"/>
+      <c r="B263" s="62"/>
+      <c r="C263" s="64"/>
       <c r="D263" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10477,13 +10417,13 @@
       <c r="N263" s="47"/>
       <c r="O263" s="47"/>
       <c r="P263" s="47"/>
-      <c r="Q263" s="66"/>
+      <c r="Q263" s="62"/>
       <c r="R263" s="60"/>
     </row>
     <row r="264" spans="1:18" ht="15.75">
       <c r="A264" s="22"/>
-      <c r="B264" s="66"/>
-      <c r="C264" s="68"/>
+      <c r="B264" s="62"/>
+      <c r="C264" s="64"/>
       <c r="D264" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10512,13 +10452,13 @@
       <c r="N264" s="47"/>
       <c r="O264" s="47"/>
       <c r="P264" s="47"/>
-      <c r="Q264" s="66"/>
+      <c r="Q264" s="62"/>
       <c r="R264" s="60"/>
     </row>
     <row r="265" spans="1:18" ht="15.75">
       <c r="A265" s="22"/>
-      <c r="B265" s="66"/>
-      <c r="C265" s="68"/>
+      <c r="B265" s="62"/>
+      <c r="C265" s="64"/>
       <c r="D265" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10547,13 +10487,13 @@
       <c r="N265" s="47"/>
       <c r="O265" s="47"/>
       <c r="P265" s="47"/>
-      <c r="Q265" s="66"/>
+      <c r="Q265" s="62"/>
       <c r="R265" s="60"/>
     </row>
     <row r="266" spans="1:18" ht="15.75">
       <c r="A266" s="22"/>
-      <c r="B266" s="66"/>
-      <c r="C266" s="68"/>
+      <c r="B266" s="62"/>
+      <c r="C266" s="64"/>
       <c r="D266" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10581,13 +10521,13 @@
       </c>
       <c r="N266" s="47"/>
       <c r="P266" s="47"/>
-      <c r="Q266" s="66"/>
+      <c r="Q266" s="62"/>
       <c r="R266" s="60"/>
     </row>
     <row r="267" spans="1:18" ht="15.75">
       <c r="A267" s="22"/>
-      <c r="B267" s="66"/>
-      <c r="C267" s="68"/>
+      <c r="B267" s="62"/>
+      <c r="C267" s="64"/>
       <c r="D267" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10616,13 +10556,13 @@
       <c r="N267" s="47"/>
       <c r="O267" s="47"/>
       <c r="P267" s="47"/>
-      <c r="Q267" s="66"/>
+      <c r="Q267" s="62"/>
       <c r="R267" s="60"/>
     </row>
     <row r="268" spans="1:18" ht="15.75">
       <c r="A268" s="22"/>
-      <c r="B268" s="66"/>
-      <c r="C268" s="68"/>
+      <c r="B268" s="62"/>
+      <c r="C268" s="64"/>
       <c r="D268" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10651,13 +10591,13 @@
       <c r="N268" s="47"/>
       <c r="O268" s="47"/>
       <c r="P268" s="47"/>
-      <c r="Q268" s="66"/>
+      <c r="Q268" s="62"/>
       <c r="R268" s="60"/>
     </row>
     <row r="269" spans="1:18" ht="15.75">
       <c r="A269" s="22"/>
-      <c r="B269" s="66"/>
-      <c r="C269" s="68"/>
+      <c r="B269" s="62"/>
+      <c r="C269" s="64"/>
       <c r="D269" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10686,13 +10626,13 @@
       <c r="N269" s="47"/>
       <c r="O269" s="47"/>
       <c r="P269" s="47"/>
-      <c r="Q269" s="66"/>
+      <c r="Q269" s="62"/>
       <c r="R269" s="60"/>
     </row>
     <row r="270" spans="1:18" ht="15.75">
       <c r="A270" s="22"/>
-      <c r="B270" s="66"/>
-      <c r="C270" s="68"/>
+      <c r="B270" s="62"/>
+      <c r="C270" s="64"/>
       <c r="D270" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10721,13 +10661,13 @@
       <c r="N270" s="47"/>
       <c r="O270" s="47"/>
       <c r="P270" s="47"/>
-      <c r="Q270" s="66"/>
+      <c r="Q270" s="62"/>
       <c r="R270" s="60"/>
     </row>
     <row r="271" spans="1:18" ht="15.75">
       <c r="A271" s="22"/>
-      <c r="B271" s="66"/>
-      <c r="C271" s="68"/>
+      <c r="B271" s="62"/>
+      <c r="C271" s="64"/>
       <c r="D271" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10756,13 +10696,13 @@
       <c r="N271" s="47"/>
       <c r="O271" s="47"/>
       <c r="P271" s="47"/>
-      <c r="Q271" s="66"/>
+      <c r="Q271" s="62"/>
       <c r="R271" s="60"/>
     </row>
     <row r="272" spans="1:18" ht="15.75">
       <c r="A272" s="22"/>
-      <c r="B272" s="66"/>
-      <c r="C272" s="68"/>
+      <c r="B272" s="62"/>
+      <c r="C272" s="64"/>
       <c r="D272" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10791,13 +10731,13 @@
       <c r="N272" s="47"/>
       <c r="O272" s="47"/>
       <c r="P272" s="47"/>
-      <c r="Q272" s="66"/>
+      <c r="Q272" s="62"/>
       <c r="R272" s="60"/>
     </row>
     <row r="273" spans="1:18" ht="15.75">
       <c r="A273" s="28"/>
-      <c r="B273" s="67"/>
-      <c r="C273" s="68"/>
+      <c r="B273" s="63"/>
+      <c r="C273" s="64"/>
       <c r="D273" s="5" t="str">
         <f t="shared" si="16"/>
         <v>-</v>
@@ -10826,7 +10766,7 @@
       <c r="N273" s="47"/>
       <c r="O273" s="47"/>
       <c r="P273" s="47"/>
-      <c r="Q273" s="67"/>
+      <c r="Q273" s="63"/>
       <c r="R273" s="60"/>
     </row>
     <row r="274" spans="1:18" ht="15.75">
@@ -10881,29 +10821,27 @@
   </sheetData>
   <autoFilter ref="A1:P273"/>
   <mergeCells count="60">
-    <mergeCell ref="A4:A33"/>
-    <mergeCell ref="A34:A78"/>
-    <mergeCell ref="A79:A108"/>
-    <mergeCell ref="B4:B18"/>
-    <mergeCell ref="B19:B33"/>
-    <mergeCell ref="B34:B48"/>
-    <mergeCell ref="B49:B63"/>
-    <mergeCell ref="B64:B78"/>
-    <mergeCell ref="B79:B93"/>
-    <mergeCell ref="B94:B108"/>
-    <mergeCell ref="B229:B243"/>
-    <mergeCell ref="B244:B258"/>
-    <mergeCell ref="B109:B123"/>
-    <mergeCell ref="B124:B138"/>
-    <mergeCell ref="B139:B153"/>
-    <mergeCell ref="B154:B168"/>
-    <mergeCell ref="B169:B183"/>
-    <mergeCell ref="C184:C198"/>
-    <mergeCell ref="C199:C213"/>
-    <mergeCell ref="C214:C228"/>
-    <mergeCell ref="B184:B198"/>
-    <mergeCell ref="B199:B213"/>
-    <mergeCell ref="B214:B228"/>
+    <mergeCell ref="R4:R93"/>
+    <mergeCell ref="R94:R273"/>
+    <mergeCell ref="A1:F2"/>
+    <mergeCell ref="Q199:Q213"/>
+    <mergeCell ref="Q214:Q228"/>
+    <mergeCell ref="Q229:Q243"/>
+    <mergeCell ref="Q244:Q258"/>
+    <mergeCell ref="Q259:Q273"/>
+    <mergeCell ref="C229:C243"/>
+    <mergeCell ref="C244:C258"/>
+    <mergeCell ref="C259:C273"/>
+    <mergeCell ref="Q4:Q18"/>
+    <mergeCell ref="Q19:Q33"/>
+    <mergeCell ref="Q34:Q48"/>
+    <mergeCell ref="Q49:Q63"/>
+    <mergeCell ref="Q64:Q78"/>
+    <mergeCell ref="Q79:Q93"/>
+    <mergeCell ref="Q94:Q108"/>
+    <mergeCell ref="Q109:Q123"/>
+    <mergeCell ref="Q124:Q138"/>
+    <mergeCell ref="Q139:Q153"/>
     <mergeCell ref="Q154:Q168"/>
     <mergeCell ref="Q169:Q183"/>
     <mergeCell ref="Q184:Q198"/>
@@ -10920,120 +10858,122 @@
     <mergeCell ref="C139:C153"/>
     <mergeCell ref="C154:C168"/>
     <mergeCell ref="C169:C183"/>
-    <mergeCell ref="Q79:Q93"/>
-    <mergeCell ref="Q94:Q108"/>
-    <mergeCell ref="Q109:Q123"/>
-    <mergeCell ref="Q124:Q138"/>
-    <mergeCell ref="Q139:Q153"/>
-    <mergeCell ref="R4:R93"/>
-    <mergeCell ref="R94:R273"/>
-    <mergeCell ref="A1:F2"/>
-    <mergeCell ref="Q199:Q213"/>
-    <mergeCell ref="Q214:Q228"/>
-    <mergeCell ref="Q229:Q243"/>
-    <mergeCell ref="Q244:Q258"/>
-    <mergeCell ref="Q259:Q273"/>
-    <mergeCell ref="C229:C243"/>
-    <mergeCell ref="C244:C258"/>
-    <mergeCell ref="C259:C273"/>
-    <mergeCell ref="Q4:Q18"/>
-    <mergeCell ref="Q19:Q33"/>
-    <mergeCell ref="Q34:Q48"/>
-    <mergeCell ref="Q49:Q63"/>
-    <mergeCell ref="Q64:Q78"/>
+    <mergeCell ref="C184:C198"/>
+    <mergeCell ref="C199:C213"/>
+    <mergeCell ref="C214:C228"/>
+    <mergeCell ref="B184:B198"/>
+    <mergeCell ref="B199:B213"/>
+    <mergeCell ref="B214:B228"/>
+    <mergeCell ref="B229:B243"/>
+    <mergeCell ref="B244:B258"/>
+    <mergeCell ref="B109:B123"/>
+    <mergeCell ref="B124:B138"/>
+    <mergeCell ref="B139:B153"/>
+    <mergeCell ref="B154:B168"/>
+    <mergeCell ref="B169:B183"/>
+    <mergeCell ref="A4:A33"/>
+    <mergeCell ref="A34:A78"/>
+    <mergeCell ref="A79:A108"/>
+    <mergeCell ref="B4:B18"/>
+    <mergeCell ref="B19:B33"/>
+    <mergeCell ref="B34:B48"/>
+    <mergeCell ref="B49:B63"/>
+    <mergeCell ref="B64:B78"/>
+    <mergeCell ref="B79:B93"/>
+    <mergeCell ref="B94:B108"/>
   </mergeCells>
   <conditionalFormatting sqref="H50">
-    <cfRule type="expression" dxfId="32" priority="4" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="4" stopIfTrue="1">
       <formula>I50="I"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="23" priority="5" stopIfTrue="1">
       <formula>I50="W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="6" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="6" stopIfTrue="1">
       <formula>I50="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H51">
-    <cfRule type="expression" dxfId="29" priority="1" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="1" stopIfTrue="1">
       <formula>I51="I"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="2" stopIfTrue="1">
+    <cfRule type="expression" dxfId="20" priority="2" stopIfTrue="1">
       <formula>I51="W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="3" stopIfTrue="1">
       <formula>I51="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D4:D273">
-    <cfRule type="containsText" dxfId="26" priority="9" operator="containsText" text="Check">
+    <cfRule type="containsText" dxfId="18" priority="9" operator="containsText" text="Check">
       <formula>NOT(ISERROR(SEARCH("Check",D4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49:H50">
-    <cfRule type="expression" dxfId="25" priority="31" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="31" stopIfTrue="1">
       <formula>I50="I"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="32" stopIfTrue="1">
       <formula>I50="W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="33" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="33" stopIfTrue="1">
       <formula>I50="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J276">
-    <cfRule type="expression" dxfId="22" priority="23" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="23" stopIfTrue="1">
       <formula>J4="N"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R4:R273">
-    <cfRule type="containsText" dxfId="21" priority="10" operator="containsText" text="NA">
+    <cfRule type="containsText" dxfId="13" priority="10" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",R4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="20" priority="11" operator="containsText" text="U">
+    <cfRule type="containsText" dxfId="12" priority="11" operator="containsText" text="U">
       <formula>NOT(ISERROR(SEARCH("U",R4)))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="24" stopIfTrue="1">
+    <cfRule type="expression" dxfId="11" priority="24" stopIfTrue="1">
       <formula>LEFT(R4,LEN("S"))="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R274:R276">
-    <cfRule type="expression" dxfId="18" priority="12" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="12" stopIfTrue="1">
       <formula>R274="U"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
       <formula>R274="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:G273">
-    <cfRule type="expression" dxfId="16" priority="21" stopIfTrue="1">
+    <cfRule type="expression" dxfId="8" priority="21" stopIfTrue="1">
       <formula>G4="Aff"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="22" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="22" stopIfTrue="1">
       <formula>G4="Doc"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H52:H276 H4:H49">
-    <cfRule type="expression" dxfId="14" priority="18" stopIfTrue="1">
+    <cfRule type="expression" dxfId="6" priority="18" stopIfTrue="1">
       <formula>I4="I"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="19" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="19" stopIfTrue="1">
       <formula>I4="W"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="20" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="20" stopIfTrue="1">
       <formula>I4="S"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N267:Q276 P266:Q266 N4:Q265 N266">
-    <cfRule type="expression" dxfId="11" priority="17" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="17" stopIfTrue="1">
       <formula>N4="FI"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="14" stopIfTrue="1">
+    <cfRule type="expression" dxfId="2" priority="14" stopIfTrue="1">
       <formula>N4="NI"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="15" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="15" stopIfTrue="1">
       <formula>N4="PI"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="16" stopIfTrue="1">
+    <cfRule type="expression" dxfId="0" priority="16" stopIfTrue="1">
       <formula>N4="LI"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11070,6 +11010,7 @@
     <hyperlink ref="E64" r:id="rId13"/>
     <hyperlink ref="E80" r:id="rId14"/>
     <hyperlink ref="E79" r:id="rId15"/>
+    <hyperlink ref="E95" r:id="rId16"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait"/>

</xml_diff>